<commit_message>
update course datasets and relevant documentation
</commit_message>
<xml_diff>
--- a/course-datasets/Data dictionary.xlsx
+++ b/course-datasets/Data dictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stepheaneff/Documents/work/GT/data-science-basics-2024/course-datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72FA1185-C0CF-4E43-BFBF-5ED64CFBC623}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B1B0C81-A792-0349-8067-0E0DCC66F33A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="460" yWindow="760" windowWidth="29780" windowHeight="16820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="205">
   <si>
     <t>Text</t>
   </si>
@@ -501,43 +501,22 @@
     <t>Data dictionary still in progress</t>
   </si>
   <si>
-    <t>measles_vaccines</t>
-  </si>
-  <si>
     <t>TBD</t>
   </si>
   <si>
-    <t>line_id</t>
-  </si>
-  <si>
     <t>country_name</t>
   </si>
   <si>
     <t>iso_code</t>
   </si>
   <si>
-    <t>vaccine_policy</t>
-  </si>
-  <si>
-    <t>Line ID</t>
-  </si>
-  <si>
     <t>Country name</t>
   </si>
   <si>
     <t>ISO code</t>
   </si>
   <si>
-    <t>Vaccine policy</t>
-  </si>
-  <si>
-    <t>Added initial data</t>
-  </si>
-  <si>
-    <t>Changed datasets</t>
-  </si>
-  <si>
-    <t>Added measles vaccine data</t>
+    <t>one row per World Health Assembly member state</t>
   </si>
   <si>
     <r>
@@ -550,35 +529,149 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>March 29, 2024</t>
+      <t>April 5, 2024</t>
     </r>
   </si>
   <si>
-    <t>countries.tsv</t>
-  </si>
-  <si>
-    <t>Country-level information, for World Health Assembly member states, including country name, ISO code, population size, and income designation</t>
-  </si>
-  <si>
-    <t>one row per World Health Assembly member state</t>
-  </si>
-  <si>
-    <t>World Health Organization. (10 February, 2023). Countries overview. World Health Organization. https://www.who.int/countries/ 
+    <t>measles_policies.tsv</t>
+  </si>
+  <si>
+    <t>Country-level information, including measles policy information, for World Health Assembly member state. Table also includes relevant information about the country including population size, region, and income designation</t>
+  </si>
+  <si>
+    <t>measles_policies</t>
+  </si>
+  <si>
+    <t>who_region</t>
+  </si>
+  <si>
+    <t>world_bank_region</t>
+  </si>
+  <si>
+    <t>income_group</t>
+  </si>
+  <si>
+    <t>total_population</t>
+  </si>
+  <si>
+    <t>pct_rural</t>
+  </si>
+  <si>
+    <t>measles_vaccine_policy</t>
+  </si>
+  <si>
+    <t>Region (WHO)</t>
+  </si>
+  <si>
+    <t>Region (World Bank)</t>
+  </si>
+  <si>
+    <t>Income group</t>
+  </si>
+  <si>
+    <t>Total population</t>
+  </si>
+  <si>
+    <t>Percent rural</t>
+  </si>
+  <si>
+    <t>Vaccine policy (measles)</t>
+  </si>
+  <si>
+    <t>measles_cases</t>
+  </si>
+  <si>
+    <t>measles_cases.tsv</t>
+  </si>
+  <si>
+    <t>one row per World Health Assembly member state per month</t>
+  </si>
+  <si>
+    <t>Country-level information, per month, on laboratory confirmed, epidemiologically linked, and/or clinical measles cases reported to the World Health Organization</t>
+  </si>
+  <si>
+    <t>World Health Organization. (10 February, 2023). Countries overview.  https://www.who.int/countries/ 
 World Bank. (29 March, 2024). World Bank Country and Lending Groups. https://datahelpdesk.worldbank.org/knowledgebase/articles/906519-world-bank-country-and-lending-groups
 World Bank. (29 March, 2024). Population estimates and projections, 2024. https://databank.worldbank.org/source/population-estimates-and-projections#</t>
   </si>
   <si>
-    <t>Updated datasets</t>
-  </si>
-  <si>
-    <t>Added country-level vaccine data</t>
+    <t>World Health Organization. (22 March, 2024). Distribution of Measles Cases by Country and Month. https://www.who.int/teams/immunization-vaccines-and-biologicals/immunization-analysis-and-insights/surveillance/monitoring/provisional-monthly-measles-and-rubella-data</t>
+  </si>
+  <si>
+    <t>month</t>
+  </si>
+  <si>
+    <t>Month</t>
+  </si>
+  <si>
+    <t>Measles cases</t>
+  </si>
+  <si>
+    <t>Number of laboratory confirmed, epidemiologically linked, and/or clinical cases as reported to the World Health Organization by the country in the specified month</t>
+  </si>
+  <si>
+    <t>The ISO code of the country</t>
+  </si>
+  <si>
+    <t>character</t>
+  </si>
+  <si>
+    <t>ISO 3166 Country Codes. https://www.iso.org/iso-3166-country-codes.html</t>
+  </si>
+  <si>
+    <t>The name of the country</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>World Bank. (29 March, 2024). World Bank Country and Lending Groups. https://datahelpdesk.worldbank.org/knowledgebase/articles/906519-world-bank-country-and-lending-groups</t>
+  </si>
+  <si>
+    <t>World Health Organization. (20 February 2023). https://www.who.int/countries</t>
+  </si>
+  <si>
+    <t>The region of the country as designated by the World Health Organization (WHO), corresponding to the WHO regional office</t>
+  </si>
+  <si>
+    <t>The region of the country as designated by the World Bank</t>
+  </si>
+  <si>
+    <t>The income group of the country as designated by the World Bank for the year 2024</t>
+  </si>
+  <si>
+    <t>numeric</t>
+  </si>
+  <si>
+    <t>The total population of the country in the year 2024, as estimated by the World Bank</t>
+  </si>
+  <si>
+    <t>The percent of the total population living in a rural area, as estimated by the World Bank for the year 2024</t>
+  </si>
+  <si>
+    <t>Whether or not the country requires measles vaccination</t>
+  </si>
+  <si>
+    <t>The month for which data are reported</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>Completed initial data dictionary</t>
+  </si>
+  <si>
+    <t>Added initial notes</t>
+  </si>
+  <si>
+    <t>Updated data dictionary, though I anticipate more changes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -649,19 +742,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -726,7 +806,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -761,10 +841,13 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -773,23 +856,31 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1082,35 +1173,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="124" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="18"/>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
+      <c r="A1" s="21"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
     </row>
     <row r="2" spans="1:22" ht="17" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="17" t="s">
         <v>150</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
     </row>
     <row r="3" spans="1:22" ht="17" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
-        <v>167</v>
-      </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
+      <c r="A3" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
     </row>
     <row r="4" spans="1:22" ht="17" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="18" t="s">
         <v>148</v>
       </c>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
     </row>
     <row r="5" spans="1:22" ht="17" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
@@ -1147,19 +1238,19 @@
     </row>
     <row r="8" spans="1:22" ht="152" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>149</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>171</v>
+        <v>180</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -1179,12 +1270,22 @@
       <c r="U8" s="2"/>
       <c r="V8" s="2"/>
     </row>
-    <row r="9" spans="1:22" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="7"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="2"/>
+    <row r="9" spans="1:22" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>181</v>
+      </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
@@ -3280,12 +3381,12 @@
     <row r="1003" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A1:E1"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="A3:D3"/>
     <mergeCell ref="A4:D4"/>
     <mergeCell ref="A6:E6"/>
     <mergeCell ref="B5:E5"/>
-    <mergeCell ref="A1:E1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -3302,17 +3403,17 @@
   <dimension ref="A1:U999"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="35.19921875" customWidth="1"/>
-    <col min="2" max="2" width="47" customWidth="1"/>
-    <col min="3" max="3" width="50.3984375" customWidth="1"/>
-    <col min="4" max="4" width="59.796875" customWidth="1"/>
+    <col min="1" max="1" width="27" customWidth="1"/>
+    <col min="2" max="2" width="36" customWidth="1"/>
+    <col min="3" max="3" width="32.796875" customWidth="1"/>
+    <col min="4" max="4" width="82.796875" style="22" customWidth="1"/>
     <col min="5" max="5" width="30" customWidth="1"/>
-    <col min="6" max="6" width="40.19921875" customWidth="1"/>
+    <col min="6" max="6" width="40.19921875" style="24" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="17" customHeight="1" x14ac:dyDescent="0.25">
@@ -3347,28 +3448,28 @@
       <c r="E3" s="12" t="s">
         <v>139</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="11" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>156</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>155</v>
+        <v>158</v>
+      </c>
+      <c r="D4" s="23" t="s">
+        <v>186</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>155</v>
-      </c>
-      <c r="F4" s="13" t="s">
-        <v>155</v>
+        <v>187</v>
+      </c>
+      <c r="F4" s="25" t="s">
+        <v>188</v>
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
@@ -3388,22 +3489,22 @@
     </row>
     <row r="5" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
       <c r="B5" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="C5" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="C5" s="8" t="s">
-        <v>161</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>155</v>
+      <c r="D5" s="23" t="s">
+        <v>189</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>155</v>
-      </c>
-      <c r="F5" s="13" t="s">
-        <v>155</v>
+        <v>187</v>
+      </c>
+      <c r="F5" s="25" t="s">
+        <v>190</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
@@ -3423,22 +3524,22 @@
     </row>
     <row r="6" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>155</v>
+        <v>170</v>
+      </c>
+      <c r="D6" s="23" t="s">
+        <v>193</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>155</v>
-      </c>
-      <c r="F6" s="13" t="s">
-        <v>155</v>
+        <v>187</v>
+      </c>
+      <c r="F6" s="25" t="s">
+        <v>192</v>
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
@@ -3458,22 +3559,22 @@
     </row>
     <row r="7" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>163</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>155</v>
+        <v>171</v>
+      </c>
+      <c r="D7" s="23" t="s">
+        <v>194</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>155</v>
-      </c>
-      <c r="F7" s="13" t="s">
-        <v>155</v>
+        <v>187</v>
+      </c>
+      <c r="F7" s="25" t="s">
+        <v>191</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
@@ -3491,13 +3592,25 @@
       <c r="T7" s="2"/>
       <c r="U7" s="2"/>
     </row>
-    <row r="8" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="8"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="14"/>
+    <row r="8" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="D8" s="23" t="s">
+        <v>195</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="F8" s="25" t="s">
+        <v>191</v>
+      </c>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
@@ -3514,13 +3627,25 @@
       <c r="T8" s="2"/>
       <c r="U8" s="2"/>
     </row>
-    <row r="9" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="8"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="14"/>
+    <row r="9" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="D9" s="23" t="s">
+        <v>197</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>196</v>
+      </c>
+      <c r="F9" s="25" t="s">
+        <v>191</v>
+      </c>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
@@ -3537,13 +3662,25 @@
       <c r="T9" s="2"/>
       <c r="U9" s="2"/>
     </row>
-    <row r="10" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="14"/>
+    <row r="10" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="D10" s="23" t="s">
+        <v>198</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>196</v>
+      </c>
+      <c r="F10" s="25" t="s">
+        <v>191</v>
+      </c>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
@@ -3560,13 +3697,25 @@
       <c r="T10" s="2"/>
       <c r="U10" s="2"/>
     </row>
-    <row r="11" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="8"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="14"/>
+    <row r="11" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="D11" s="23" t="s">
+        <v>199</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>196</v>
+      </c>
+      <c r="F11" s="25" t="s">
+        <v>154</v>
+      </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
@@ -3583,13 +3732,25 @@
       <c r="T11" s="2"/>
       <c r="U11" s="2"/>
     </row>
-    <row r="12" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
+    <row r="12" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="D12" s="23" t="s">
+        <v>186</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="F12" s="25" t="s">
+        <v>188</v>
+      </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
@@ -3606,13 +3767,25 @@
       <c r="T12" s="2"/>
       <c r="U12" s="2"/>
     </row>
-    <row r="13" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
+    <row r="13" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="D13" s="23" t="s">
+        <v>189</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="F13" s="25" t="s">
+        <v>190</v>
+      </c>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
@@ -3629,13 +3802,25 @@
       <c r="T13" s="2"/>
       <c r="U13" s="2"/>
     </row>
-    <row r="14" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
+    <row r="14" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="D14" s="23" t="s">
+        <v>200</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="F14" s="26" t="s">
+        <v>181</v>
+      </c>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
@@ -3652,13 +3837,25 @@
       <c r="T14" s="2"/>
       <c r="U14" s="2"/>
     </row>
-    <row r="15" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
+    <row r="15" spans="1:21" ht="70" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>196</v>
+      </c>
+      <c r="F15" s="26" t="s">
+        <v>181</v>
+      </c>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
@@ -3681,7 +3878,7 @@
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
+      <c r="F16" s="27"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
@@ -3704,7 +3901,7 @@
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
+      <c r="F17" s="27"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
@@ -3727,7 +3924,7 @@
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
+      <c r="F18" s="27"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
@@ -3750,7 +3947,7 @@
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
+      <c r="F19" s="27"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
@@ -3773,7 +3970,7 @@
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
+      <c r="F20" s="27"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
@@ -3796,7 +3993,7 @@
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
+      <c r="F21" s="27"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
@@ -3819,7 +4016,7 @@
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
+      <c r="F22" s="27"/>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
@@ -3842,7 +4039,7 @@
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
+      <c r="F23" s="27"/>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
@@ -3865,7 +4062,7 @@
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
+      <c r="F24" s="27"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
@@ -3888,7 +4085,7 @@
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
+      <c r="F25" s="27"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
@@ -3911,7 +4108,7 @@
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
+      <c r="F26" s="27"/>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
@@ -3934,7 +4131,7 @@
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
+      <c r="F27" s="27"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
@@ -3957,7 +4154,7 @@
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
+      <c r="F28" s="27"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
@@ -3980,7 +4177,7 @@
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
+      <c r="F29" s="27"/>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
@@ -4003,7 +4200,7 @@
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
+      <c r="F30" s="27"/>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
@@ -4026,7 +4223,7 @@
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
+      <c r="F31" s="27"/>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
@@ -4049,7 +4246,7 @@
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
-      <c r="F32" s="3"/>
+      <c r="F32" s="28"/>
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
       <c r="I32" s="3"/>
@@ -4072,7 +4269,7 @@
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
-      <c r="F33" s="3"/>
+      <c r="F33" s="28"/>
       <c r="G33" s="3"/>
       <c r="H33" s="3"/>
       <c r="I33" s="3"/>
@@ -4095,7 +4292,7 @@
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>
-      <c r="F34" s="3"/>
+      <c r="F34" s="28"/>
       <c r="G34" s="3"/>
       <c r="H34" s="3"/>
       <c r="I34" s="3"/>
@@ -4118,7 +4315,7 @@
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
       <c r="E35" s="3"/>
-      <c r="F35" s="3"/>
+      <c r="F35" s="28"/>
       <c r="G35" s="3"/>
       <c r="H35" s="3"/>
       <c r="I35" s="3"/>
@@ -4141,7 +4338,7 @@
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
-      <c r="F36" s="3"/>
+      <c r="F36" s="28"/>
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
       <c r="I36" s="3"/>
@@ -4164,7 +4361,7 @@
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
-      <c r="F37" s="3"/>
+      <c r="F37" s="28"/>
       <c r="G37" s="3"/>
       <c r="H37" s="3"/>
       <c r="I37" s="3"/>
@@ -4187,7 +4384,7 @@
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
-      <c r="F38" s="3"/>
+      <c r="F38" s="28"/>
       <c r="G38" s="3"/>
       <c r="H38" s="3"/>
       <c r="I38" s="3"/>
@@ -4210,7 +4407,7 @@
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
       <c r="E39" s="3"/>
-      <c r="F39" s="3"/>
+      <c r="F39" s="28"/>
       <c r="G39" s="3"/>
       <c r="H39" s="3"/>
       <c r="I39" s="3"/>
@@ -4233,7 +4430,7 @@
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
       <c r="E40" s="3"/>
-      <c r="F40" s="3"/>
+      <c r="F40" s="28"/>
       <c r="G40" s="3"/>
       <c r="H40" s="3"/>
       <c r="I40" s="3"/>
@@ -4256,7 +4453,7 @@
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
       <c r="E41" s="3"/>
-      <c r="F41" s="3"/>
+      <c r="F41" s="28"/>
       <c r="G41" s="3"/>
       <c r="H41" s="3"/>
       <c r="I41" s="3"/>
@@ -4279,7 +4476,7 @@
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
       <c r="E42" s="3"/>
-      <c r="F42" s="3"/>
+      <c r="F42" s="28"/>
       <c r="G42" s="3"/>
       <c r="H42" s="3"/>
       <c r="I42" s="3"/>
@@ -4302,7 +4499,7 @@
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
       <c r="E43" s="3"/>
-      <c r="F43" s="3"/>
+      <c r="F43" s="28"/>
       <c r="G43" s="3"/>
       <c r="H43" s="3"/>
       <c r="I43" s="3"/>
@@ -4325,7 +4522,7 @@
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
       <c r="E44" s="3"/>
-      <c r="F44" s="3"/>
+      <c r="F44" s="28"/>
       <c r="G44" s="3"/>
       <c r="H44" s="3"/>
       <c r="I44" s="3"/>
@@ -4348,7 +4545,7 @@
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
       <c r="E45" s="3"/>
-      <c r="F45" s="3"/>
+      <c r="F45" s="28"/>
       <c r="G45" s="3"/>
       <c r="H45" s="3"/>
       <c r="I45" s="3"/>
@@ -4371,7 +4568,7 @@
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
       <c r="E46" s="3"/>
-      <c r="F46" s="3"/>
+      <c r="F46" s="28"/>
       <c r="G46" s="3"/>
       <c r="H46" s="3"/>
       <c r="I46" s="3"/>
@@ -4394,7 +4591,7 @@
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
       <c r="E47" s="3"/>
-      <c r="F47" s="3"/>
+      <c r="F47" s="28"/>
       <c r="G47" s="3"/>
       <c r="H47" s="3"/>
       <c r="I47" s="3"/>
@@ -4417,7 +4614,7 @@
       <c r="C48" s="3"/>
       <c r="D48" s="3"/>
       <c r="E48" s="3"/>
-      <c r="F48" s="3"/>
+      <c r="F48" s="28"/>
       <c r="G48" s="3"/>
       <c r="H48" s="3"/>
       <c r="I48" s="3"/>
@@ -4440,7 +4637,7 @@
       <c r="C49" s="3"/>
       <c r="D49" s="3"/>
       <c r="E49" s="3"/>
-      <c r="F49" s="3"/>
+      <c r="F49" s="28"/>
       <c r="G49" s="3"/>
       <c r="H49" s="3"/>
       <c r="I49" s="3"/>
@@ -4463,7 +4660,7 @@
       <c r="C50" s="3"/>
       <c r="D50" s="3"/>
       <c r="E50" s="3"/>
-      <c r="F50" s="3"/>
+      <c r="F50" s="28"/>
       <c r="G50" s="3"/>
       <c r="H50" s="3"/>
       <c r="I50" s="3"/>
@@ -4486,7 +4683,7 @@
       <c r="C51" s="3"/>
       <c r="D51" s="3"/>
       <c r="E51" s="3"/>
-      <c r="F51" s="3"/>
+      <c r="F51" s="28"/>
       <c r="G51" s="3"/>
       <c r="H51" s="3"/>
       <c r="I51" s="3"/>
@@ -4509,7 +4706,7 @@
       <c r="C52" s="3"/>
       <c r="D52" s="3"/>
       <c r="E52" s="3"/>
-      <c r="F52" s="3"/>
+      <c r="F52" s="28"/>
       <c r="G52" s="3"/>
       <c r="H52" s="3"/>
       <c r="I52" s="3"/>
@@ -5491,7 +5688,7 @@
   <dimension ref="A1:S999"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -7524,10 +7721,10 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:S999"/>
+  <dimension ref="A1:S997"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -7570,19 +7767,19 @@
       </c>
     </row>
     <row r="4" spans="1:19" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="21">
+      <c r="A4" s="15">
         <v>45310</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="16" t="s">
         <v>151</v>
       </c>
-      <c r="C4" s="22" t="s">
-        <v>164</v>
-      </c>
-      <c r="D4" s="22" t="s">
+      <c r="C4" s="16" t="s">
+        <v>203</v>
+      </c>
+      <c r="D4" s="16" t="s">
         <v>152</v>
       </c>
-      <c r="E4" s="22" t="s">
+      <c r="E4" s="16" t="s">
         <v>153</v>
       </c>
       <c r="F4" s="2"/>
@@ -7601,19 +7798,19 @@
       <c r="S4" s="2"/>
     </row>
     <row r="5" spans="1:19" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="21">
-        <v>45373</v>
-      </c>
-      <c r="B5" s="22" t="s">
-        <v>165</v>
-      </c>
-      <c r="C5" s="23" t="s">
-        <v>166</v>
-      </c>
-      <c r="D5" s="23" t="s">
+      <c r="A5" s="14">
+        <v>45387</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>202</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>204</v>
+      </c>
+      <c r="D5" s="16" t="s">
         <v>152</v>
       </c>
-      <c r="E5" s="22" t="s">
+      <c r="E5" s="16" t="s">
         <v>153</v>
       </c>
       <c r="F5" s="2"/>
@@ -7632,21 +7829,11 @@
       <c r="S5" s="2"/>
     </row>
     <row r="6" spans="1:19" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="15">
-        <v>45380</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>172</v>
-      </c>
-      <c r="C6" s="23" t="s">
-        <v>173</v>
-      </c>
-      <c r="D6" s="23" t="s">
-        <v>152</v>
-      </c>
-      <c r="E6" s="22" t="s">
-        <v>153</v>
-      </c>
+      <c r="A6" s="7"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
@@ -7684,8 +7871,8 @@
       <c r="S7" s="2"/>
     </row>
     <row r="8" spans="1:19" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="7"/>
-      <c r="B8" s="8"/>
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -7705,8 +7892,8 @@
       <c r="S8" s="2"/>
     </row>
     <row r="9" spans="1:19" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="7"/>
-      <c r="B9" s="8"/>
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
@@ -7726,8 +7913,8 @@
       <c r="S9" s="2"/>
     </row>
     <row r="10" spans="1:19" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -7747,8 +7934,8 @@
       <c r="S10" s="2"/>
     </row>
     <row r="11" spans="1:19" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
@@ -8146,46 +8333,46 @@
       <c r="S29" s="2"/>
     </row>
     <row r="30" spans="1:19" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="2"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
-      <c r="H30" s="2"/>
-      <c r="I30" s="2"/>
-      <c r="J30" s="2"/>
-      <c r="K30" s="2"/>
-      <c r="L30" s="2"/>
-      <c r="M30" s="2"/>
-      <c r="N30" s="2"/>
-      <c r="O30" s="2"/>
-      <c r="P30" s="2"/>
-      <c r="Q30" s="2"/>
-      <c r="R30" s="2"/>
-      <c r="S30" s="2"/>
+      <c r="A30" s="3"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="3"/>
+      <c r="J30" s="3"/>
+      <c r="K30" s="3"/>
+      <c r="L30" s="3"/>
+      <c r="M30" s="3"/>
+      <c r="N30" s="3"/>
+      <c r="O30" s="3"/>
+      <c r="P30" s="3"/>
+      <c r="Q30" s="3"/>
+      <c r="R30" s="3"/>
+      <c r="S30" s="3"/>
     </row>
     <row r="31" spans="1:19" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="2"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
-      <c r="H31" s="2"/>
-      <c r="I31" s="2"/>
-      <c r="J31" s="2"/>
-      <c r="K31" s="2"/>
-      <c r="L31" s="2"/>
-      <c r="M31" s="2"/>
-      <c r="N31" s="2"/>
-      <c r="O31" s="2"/>
-      <c r="P31" s="2"/>
-      <c r="Q31" s="2"/>
-      <c r="R31" s="2"/>
-      <c r="S31" s="2"/>
+      <c r="A31" s="3"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="3"/>
+      <c r="J31" s="3"/>
+      <c r="K31" s="3"/>
+      <c r="L31" s="3"/>
+      <c r="M31" s="3"/>
+      <c r="N31" s="3"/>
+      <c r="O31" s="3"/>
+      <c r="P31" s="3"/>
+      <c r="Q31" s="3"/>
+      <c r="R31" s="3"/>
+      <c r="S31" s="3"/>
     </row>
     <row r="32" spans="1:19" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="3"/>
@@ -8544,7 +8731,7 @@
       <c r="R48" s="3"/>
       <c r="S48" s="3"/>
     </row>
-    <row r="49" spans="1:19" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="3"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
@@ -8565,7 +8752,7 @@
       <c r="R49" s="3"/>
       <c r="S49" s="3"/>
     </row>
-    <row r="50" spans="1:19" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="3"/>
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>
@@ -8586,48 +8773,8 @@
       <c r="R50" s="3"/>
       <c r="S50" s="3"/>
     </row>
-    <row r="51" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="3"/>
-      <c r="B51" s="3"/>
-      <c r="C51" s="3"/>
-      <c r="D51" s="3"/>
-      <c r="E51" s="3"/>
-      <c r="F51" s="3"/>
-      <c r="G51" s="3"/>
-      <c r="H51" s="3"/>
-      <c r="I51" s="3"/>
-      <c r="J51" s="3"/>
-      <c r="K51" s="3"/>
-      <c r="L51" s="3"/>
-      <c r="M51" s="3"/>
-      <c r="N51" s="3"/>
-      <c r="O51" s="3"/>
-      <c r="P51" s="3"/>
-      <c r="Q51" s="3"/>
-      <c r="R51" s="3"/>
-      <c r="S51" s="3"/>
-    </row>
-    <row r="52" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="3"/>
-      <c r="B52" s="3"/>
-      <c r="C52" s="3"/>
-      <c r="D52" s="3"/>
-      <c r="E52" s="3"/>
-      <c r="F52" s="3"/>
-      <c r="G52" s="3"/>
-      <c r="H52" s="3"/>
-      <c r="I52" s="3"/>
-      <c r="J52" s="3"/>
-      <c r="K52" s="3"/>
-      <c r="L52" s="3"/>
-      <c r="M52" s="3"/>
-      <c r="N52" s="3"/>
-      <c r="O52" s="3"/>
-      <c r="P52" s="3"/>
-      <c r="Q52" s="3"/>
-      <c r="R52" s="3"/>
-      <c r="S52" s="3"/>
-    </row>
+    <row r="51" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="52" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="53" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="54" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="55" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -9573,8 +9720,6 @@
     <row r="995" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="996" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A2:E2"/>

</xml_diff>

<commit_message>
add new dataset on measles vaccine coverage
</commit_message>
<xml_diff>
--- a/course-datasets/Data dictionary.xlsx
+++ b/course-datasets/Data dictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stepheaneff/Documents/work/GT/data-science-basics-2024/course-datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B1B0C81-A792-0349-8067-0E0DCC66F33A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ABEEED7-767A-3C4C-A81A-EA65D934A1FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="460" yWindow="760" windowWidth="29780" windowHeight="16820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="460" yWindow="760" windowWidth="29780" windowHeight="16820" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table information" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="208">
   <si>
     <t>Text</t>
   </si>
@@ -499,9 +499,6 @@
   </si>
   <si>
     <t>Data dictionary still in progress</t>
-  </si>
-  <si>
-    <t>TBD</t>
   </si>
   <si>
     <t>country_name</t>
@@ -533,15 +530,6 @@
     </r>
   </si>
   <si>
-    <t>measles_policies.tsv</t>
-  </si>
-  <si>
-    <t>Country-level information, including measles policy information, for World Health Assembly member state. Table also includes relevant information about the country including population size, region, and income designation</t>
-  </si>
-  <si>
-    <t>measles_policies</t>
-  </si>
-  <si>
     <t>who_region</t>
   </si>
   <si>
@@ -665,6 +653,27 @@
   </si>
   <si>
     <t>Updated data dictionary, though I anticipate more changes</t>
+  </si>
+  <si>
+    <t>Country-level information, including measles policy and vaccine coverage information, for World Health Assembly member states. Table also includes relevant information about the country including population size, region, and income designation</t>
+  </si>
+  <si>
+    <t>mcv1_coverage</t>
+  </si>
+  <si>
+    <t>Vaccine coverage (MCV1)</t>
+  </si>
+  <si>
+    <t>Internal GHSS research</t>
+  </si>
+  <si>
+    <t>World Health Organization. (5 April 2024). Measles-containing-vaccine first-dose (MCV1) immunization coverage among 1-year-olds (%). https://www.who.int/data/gho/data/indicators/indicator-details/GHO/measles-containing-vaccine-first-dose-(mcv1)-immunization-coverage-among-1-year-olds-(-)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The percentage of children under one year of age who have received at least one dose of measles-containing vaccine in a given year. For countries recommending the first dose of measles vaccine in children over 12 months of age, the indicator is calculated as the proportion of children less than 12-23 months of age receiving one dose of measles-containing vaccine. </t>
+  </si>
+  <si>
+    <t>countries.tsv</t>
   </si>
 </sst>
 </file>
@@ -806,7 +815,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -840,7 +849,6 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -849,6 +857,27 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -862,25 +891,8 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1159,8 +1171,8 @@
   </sheetPr>
   <dimension ref="A1:V1003"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1173,51 +1185,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="124" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="21"/>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
+      <c r="A1" s="22"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
     </row>
     <row r="2" spans="1:22" ht="17" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="23" t="s">
         <v>150</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
     </row>
     <row r="3" spans="1:22" ht="17" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="18" t="s">
-        <v>160</v>
-      </c>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
+      <c r="A3" s="24" t="s">
+        <v>159</v>
+      </c>
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
     </row>
     <row r="4" spans="1:22" ht="17" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="24" t="s">
         <v>148</v>
       </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
     </row>
     <row r="5" spans="1:22" ht="17" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
-      <c r="B5" s="20"/>
-      <c r="C5" s="20"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
+      <c r="B5" s="26"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
     </row>
     <row r="6" spans="1:22" ht="37" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="25" t="s">
         <v>132</v>
       </c>
-      <c r="B6" s="19"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
     </row>
     <row r="7" spans="1:22" ht="32.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
@@ -1238,19 +1250,19 @@
     </row>
     <row r="8" spans="1:22" ht="152" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
-        <v>161</v>
+        <v>207</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>162</v>
+        <v>201</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>149</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -1272,19 +1284,19 @@
     </row>
     <row r="9" spans="1:22" ht="100" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="D9" s="9" t="s">
         <v>149</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -3400,37 +3412,38 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:U999"/>
+  <dimension ref="A1:U1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27" customWidth="1"/>
-    <col min="2" max="2" width="36" customWidth="1"/>
-    <col min="3" max="3" width="32.796875" customWidth="1"/>
-    <col min="4" max="4" width="82.796875" style="22" customWidth="1"/>
-    <col min="5" max="5" width="30" customWidth="1"/>
-    <col min="6" max="6" width="40.19921875" style="24" customWidth="1"/>
+    <col min="1" max="1" width="27" style="18" customWidth="1"/>
+    <col min="2" max="2" width="36" style="18" customWidth="1"/>
+    <col min="3" max="3" width="32.796875" style="18" customWidth="1"/>
+    <col min="4" max="4" width="82.796875" style="21" customWidth="1"/>
+    <col min="5" max="5" width="30" style="18" customWidth="1"/>
+    <col min="6" max="6" width="40.19921875" style="18" customWidth="1"/>
+    <col min="7" max="16384" width="14.3984375" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="17" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6"/>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-    </row>
-    <row r="2" spans="1:21" ht="37" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="19" t="s">
+    <row r="1" spans="1:21" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="8"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+    </row>
+    <row r="2" spans="1:21" ht="37" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="27" t="s">
         <v>137</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
     </row>
     <row r="3" spans="1:21" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
@@ -3452,24 +3465,24 @@
         <v>143</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
-        <v>163</v>
+        <v>207</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>158</v>
-      </c>
-      <c r="D4" s="23" t="s">
-        <v>186</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>187</v>
-      </c>
-      <c r="F4" s="25" t="s">
-        <v>188</v>
+        <v>157</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>182</v>
+      </c>
+      <c r="E4" s="20" t="s">
+        <v>183</v>
+      </c>
+      <c r="F4" s="20" t="s">
+        <v>184</v>
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
@@ -3487,24 +3500,24 @@
       <c r="T4" s="2"/>
       <c r="U4" s="2"/>
     </row>
-    <row r="5" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
-        <v>163</v>
+        <v>207</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>157</v>
-      </c>
-      <c r="D5" s="23" t="s">
-        <v>189</v>
-      </c>
-      <c r="E5" s="13" t="s">
-        <v>187</v>
-      </c>
-      <c r="F5" s="25" t="s">
-        <v>190</v>
+        <v>156</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>185</v>
+      </c>
+      <c r="E5" s="20" t="s">
+        <v>183</v>
+      </c>
+      <c r="F5" s="20" t="s">
+        <v>186</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
@@ -3522,24 +3535,24 @@
       <c r="T5" s="2"/>
       <c r="U5" s="2"/>
     </row>
-    <row r="6" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
-        <v>163</v>
+        <v>207</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>170</v>
-      </c>
-      <c r="D6" s="23" t="s">
-        <v>193</v>
-      </c>
-      <c r="E6" s="13" t="s">
-        <v>187</v>
-      </c>
-      <c r="F6" s="25" t="s">
-        <v>192</v>
+        <v>166</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>189</v>
+      </c>
+      <c r="E6" s="20" t="s">
+        <v>183</v>
+      </c>
+      <c r="F6" s="20" t="s">
+        <v>188</v>
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
@@ -3557,24 +3570,24 @@
       <c r="T6" s="2"/>
       <c r="U6" s="2"/>
     </row>
-    <row r="7" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
-        <v>163</v>
+        <v>207</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="D7" s="23" t="s">
-        <v>194</v>
-      </c>
-      <c r="E7" s="13" t="s">
+        <v>167</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>190</v>
+      </c>
+      <c r="E7" s="20" t="s">
+        <v>183</v>
+      </c>
+      <c r="F7" s="20" t="s">
         <v>187</v>
-      </c>
-      <c r="F7" s="25" t="s">
-        <v>191</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
@@ -3592,24 +3605,24 @@
       <c r="T7" s="2"/>
       <c r="U7" s="2"/>
     </row>
-    <row r="8" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
-        <v>163</v>
+        <v>207</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>172</v>
-      </c>
-      <c r="D8" s="23" t="s">
-        <v>195</v>
-      </c>
-      <c r="E8" s="13" t="s">
+        <v>168</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>191</v>
+      </c>
+      <c r="E8" s="20" t="s">
+        <v>183</v>
+      </c>
+      <c r="F8" s="20" t="s">
         <v>187</v>
-      </c>
-      <c r="F8" s="25" t="s">
-        <v>191</v>
       </c>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
@@ -3627,24 +3640,24 @@
       <c r="T8" s="2"/>
       <c r="U8" s="2"/>
     </row>
-    <row r="9" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="B9" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="B9" s="8" t="s">
-        <v>167</v>
-      </c>
       <c r="C9" s="8" t="s">
-        <v>173</v>
-      </c>
-      <c r="D9" s="23" t="s">
-        <v>197</v>
-      </c>
-      <c r="E9" s="13" t="s">
-        <v>196</v>
-      </c>
-      <c r="F9" s="25" t="s">
-        <v>191</v>
+        <v>169</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>193</v>
+      </c>
+      <c r="E9" s="20" t="s">
+        <v>192</v>
+      </c>
+      <c r="F9" s="20" t="s">
+        <v>187</v>
       </c>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
@@ -3662,24 +3675,24 @@
       <c r="T9" s="2"/>
       <c r="U9" s="2"/>
     </row>
-    <row r="10" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
-        <v>163</v>
+        <v>207</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>174</v>
-      </c>
-      <c r="D10" s="23" t="s">
-        <v>198</v>
-      </c>
-      <c r="E10" s="13" t="s">
-        <v>196</v>
-      </c>
-      <c r="F10" s="25" t="s">
-        <v>191</v>
+        <v>170</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>194</v>
+      </c>
+      <c r="E10" s="20" t="s">
+        <v>192</v>
+      </c>
+      <c r="F10" s="20" t="s">
+        <v>187</v>
       </c>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
@@ -3697,24 +3710,24 @@
       <c r="T10" s="2"/>
       <c r="U10" s="2"/>
     </row>
-    <row r="11" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
-        <v>163</v>
+        <v>207</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>175</v>
-      </c>
-      <c r="D11" s="23" t="s">
-        <v>199</v>
-      </c>
-      <c r="E11" s="13" t="s">
-        <v>196</v>
-      </c>
-      <c r="F11" s="25" t="s">
-        <v>154</v>
+        <v>171</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>195</v>
+      </c>
+      <c r="E11" s="20" t="s">
+        <v>192</v>
+      </c>
+      <c r="F11" s="20" t="s">
+        <v>204</v>
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
@@ -3732,24 +3745,24 @@
       <c r="T11" s="2"/>
       <c r="U11" s="2"/>
     </row>
-    <row r="12" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" ht="123" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
-        <v>176</v>
+        <v>207</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>158</v>
-      </c>
-      <c r="D12" s="23" t="s">
-        <v>186</v>
-      </c>
-      <c r="E12" s="13" t="s">
-        <v>187</v>
-      </c>
-      <c r="F12" s="25" t="s">
-        <v>188</v>
+        <v>202</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>206</v>
+      </c>
+      <c r="E12" s="20" t="s">
+        <v>192</v>
+      </c>
+      <c r="F12" s="20" t="s">
+        <v>205</v>
       </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
@@ -3767,24 +3780,24 @@
       <c r="T12" s="2"/>
       <c r="U12" s="2"/>
     </row>
-    <row r="13" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B13" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="D13" s="23" t="s">
-        <v>189</v>
-      </c>
-      <c r="E13" s="13" t="s">
-        <v>187</v>
-      </c>
-      <c r="F13" s="25" t="s">
-        <v>190</v>
+      <c r="D13" s="19" t="s">
+        <v>182</v>
+      </c>
+      <c r="E13" s="20" t="s">
+        <v>183</v>
+      </c>
+      <c r="F13" s="20" t="s">
+        <v>184</v>
       </c>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
@@ -3802,24 +3815,24 @@
       <c r="T13" s="2"/>
       <c r="U13" s="2"/>
     </row>
-    <row r="14" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>182</v>
+        <v>154</v>
       </c>
       <c r="C14" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="D14" s="19" t="s">
+        <v>185</v>
+      </c>
+      <c r="E14" s="20" t="s">
         <v>183</v>
       </c>
-      <c r="D14" s="23" t="s">
-        <v>200</v>
-      </c>
-      <c r="E14" s="13" t="s">
-        <v>201</v>
-      </c>
-      <c r="F14" s="26" t="s">
-        <v>181</v>
+      <c r="F14" s="20" t="s">
+        <v>186</v>
       </c>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
@@ -3837,24 +3850,24 @@
       <c r="T14" s="2"/>
       <c r="U14" s="2"/>
     </row>
-    <row r="15" spans="1:21" ht="70" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>184</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="E15" s="13" t="s">
+        <v>179</v>
+      </c>
+      <c r="D15" s="19" t="s">
         <v>196</v>
       </c>
-      <c r="F15" s="26" t="s">
-        <v>181</v>
+      <c r="E15" s="20" t="s">
+        <v>197</v>
+      </c>
+      <c r="F15" s="16" t="s">
+        <v>177</v>
       </c>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
@@ -3872,13 +3885,25 @@
       <c r="T15" s="2"/>
       <c r="U15" s="2"/>
     </row>
-    <row r="16" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="27"/>
+    <row r="16" spans="1:21" ht="70" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="E16" s="20" t="s">
+        <v>192</v>
+      </c>
+      <c r="F16" s="16" t="s">
+        <v>177</v>
+      </c>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
@@ -3901,7 +3926,7 @@
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
-      <c r="F17" s="27"/>
+      <c r="F17" s="17"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
@@ -3924,7 +3949,7 @@
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
-      <c r="F18" s="27"/>
+      <c r="F18" s="17"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
@@ -3947,7 +3972,7 @@
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
-      <c r="F19" s="27"/>
+      <c r="F19" s="17"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
@@ -3970,7 +3995,7 @@
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
-      <c r="F20" s="27"/>
+      <c r="F20" s="17"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
@@ -3993,7 +4018,7 @@
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
-      <c r="F21" s="27"/>
+      <c r="F21" s="17"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
@@ -4016,7 +4041,7 @@
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
-      <c r="F22" s="27"/>
+      <c r="F22" s="17"/>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
@@ -4039,7 +4064,7 @@
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
-      <c r="F23" s="27"/>
+      <c r="F23" s="17"/>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
@@ -4062,7 +4087,7 @@
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
-      <c r="F24" s="27"/>
+      <c r="F24" s="17"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
@@ -4085,7 +4110,7 @@
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
-      <c r="F25" s="27"/>
+      <c r="F25" s="17"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
@@ -4108,7 +4133,7 @@
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
-      <c r="F26" s="27"/>
+      <c r="F26" s="17"/>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
@@ -4131,7 +4156,7 @@
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
-      <c r="F27" s="27"/>
+      <c r="F27" s="17"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
@@ -4154,7 +4179,7 @@
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
-      <c r="F28" s="27"/>
+      <c r="F28" s="17"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
@@ -4177,7 +4202,7 @@
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
-      <c r="F29" s="27"/>
+      <c r="F29" s="17"/>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
@@ -4200,7 +4225,7 @@
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
-      <c r="F30" s="27"/>
+      <c r="F30" s="17"/>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
@@ -4223,7 +4248,7 @@
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
-      <c r="F31" s="27"/>
+      <c r="F31" s="17"/>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
@@ -4241,489 +4266,511 @@
       <c r="U31" s="2"/>
     </row>
     <row r="32" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="3"/>
-      <c r="B32" s="3"/>
-      <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3"/>
-      <c r="F32" s="28"/>
-      <c r="G32" s="3"/>
-      <c r="H32" s="3"/>
-      <c r="I32" s="3"/>
-      <c r="J32" s="3"/>
-      <c r="K32" s="3"/>
-      <c r="L32" s="3"/>
-      <c r="M32" s="3"/>
-      <c r="N32" s="3"/>
-      <c r="O32" s="3"/>
-      <c r="P32" s="3"/>
-      <c r="Q32" s="3"/>
-      <c r="R32" s="3"/>
-      <c r="S32" s="3"/>
-      <c r="T32" s="3"/>
-      <c r="U32" s="3"/>
+      <c r="A32" s="2"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="17"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
+      <c r="J32" s="2"/>
+      <c r="K32" s="2"/>
+      <c r="L32" s="2"/>
+      <c r="M32" s="2"/>
+      <c r="N32" s="2"/>
+      <c r="O32" s="2"/>
+      <c r="P32" s="2"/>
+      <c r="Q32" s="2"/>
+      <c r="R32" s="2"/>
+      <c r="S32" s="2"/>
+      <c r="T32" s="2"/>
+      <c r="U32" s="2"/>
     </row>
     <row r="33" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="3"/>
-      <c r="B33" s="3"/>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
-      <c r="F33" s="28"/>
-      <c r="G33" s="3"/>
-      <c r="H33" s="3"/>
-      <c r="I33" s="3"/>
-      <c r="J33" s="3"/>
-      <c r="K33" s="3"/>
-      <c r="L33" s="3"/>
-      <c r="M33" s="3"/>
-      <c r="N33" s="3"/>
-      <c r="O33" s="3"/>
-      <c r="P33" s="3"/>
-      <c r="Q33" s="3"/>
-      <c r="R33" s="3"/>
-      <c r="S33" s="3"/>
-      <c r="T33" s="3"/>
-      <c r="U33" s="3"/>
+      <c r="A33" s="2"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="17"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
+      <c r="J33" s="2"/>
+      <c r="K33" s="2"/>
+      <c r="L33" s="2"/>
+      <c r="M33" s="2"/>
+      <c r="N33" s="2"/>
+      <c r="O33" s="2"/>
+      <c r="P33" s="2"/>
+      <c r="Q33" s="2"/>
+      <c r="R33" s="2"/>
+      <c r="S33" s="2"/>
+      <c r="T33" s="2"/>
+      <c r="U33" s="2"/>
     </row>
     <row r="34" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="3"/>
-      <c r="B34" s="3"/>
-      <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
-      <c r="E34" s="3"/>
-      <c r="F34" s="28"/>
-      <c r="G34" s="3"/>
-      <c r="H34" s="3"/>
-      <c r="I34" s="3"/>
-      <c r="J34" s="3"/>
-      <c r="K34" s="3"/>
-      <c r="L34" s="3"/>
-      <c r="M34" s="3"/>
-      <c r="N34" s="3"/>
-      <c r="O34" s="3"/>
-      <c r="P34" s="3"/>
-      <c r="Q34" s="3"/>
-      <c r="R34" s="3"/>
-      <c r="S34" s="3"/>
-      <c r="T34" s="3"/>
-      <c r="U34" s="3"/>
+      <c r="A34" s="2"/>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="17"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="2"/>
+      <c r="J34" s="2"/>
+      <c r="K34" s="2"/>
+      <c r="L34" s="2"/>
+      <c r="M34" s="2"/>
+      <c r="N34" s="2"/>
+      <c r="O34" s="2"/>
+      <c r="P34" s="2"/>
+      <c r="Q34" s="2"/>
+      <c r="R34" s="2"/>
+      <c r="S34" s="2"/>
+      <c r="T34" s="2"/>
+      <c r="U34" s="2"/>
     </row>
     <row r="35" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="3"/>
-      <c r="B35" s="3"/>
-      <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
-      <c r="E35" s="3"/>
-      <c r="F35" s="28"/>
-      <c r="G35" s="3"/>
-      <c r="H35" s="3"/>
-      <c r="I35" s="3"/>
-      <c r="J35" s="3"/>
-      <c r="K35" s="3"/>
-      <c r="L35" s="3"/>
-      <c r="M35" s="3"/>
-      <c r="N35" s="3"/>
-      <c r="O35" s="3"/>
-      <c r="P35" s="3"/>
-      <c r="Q35" s="3"/>
-      <c r="R35" s="3"/>
-      <c r="S35" s="3"/>
-      <c r="T35" s="3"/>
-      <c r="U35" s="3"/>
+      <c r="A35" s="2"/>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="17"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="2"/>
+      <c r="K35" s="2"/>
+      <c r="L35" s="2"/>
+      <c r="M35" s="2"/>
+      <c r="N35" s="2"/>
+      <c r="O35" s="2"/>
+      <c r="P35" s="2"/>
+      <c r="Q35" s="2"/>
+      <c r="R35" s="2"/>
+      <c r="S35" s="2"/>
+      <c r="T35" s="2"/>
+      <c r="U35" s="2"/>
     </row>
     <row r="36" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="3"/>
-      <c r="B36" s="3"/>
-      <c r="C36" s="3"/>
-      <c r="D36" s="3"/>
-      <c r="E36" s="3"/>
-      <c r="F36" s="28"/>
-      <c r="G36" s="3"/>
-      <c r="H36" s="3"/>
-      <c r="I36" s="3"/>
-      <c r="J36" s="3"/>
-      <c r="K36" s="3"/>
-      <c r="L36" s="3"/>
-      <c r="M36" s="3"/>
-      <c r="N36" s="3"/>
-      <c r="O36" s="3"/>
-      <c r="P36" s="3"/>
-      <c r="Q36" s="3"/>
-      <c r="R36" s="3"/>
-      <c r="S36" s="3"/>
-      <c r="T36" s="3"/>
-      <c r="U36" s="3"/>
+      <c r="A36" s="2"/>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="17"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
+      <c r="J36" s="2"/>
+      <c r="K36" s="2"/>
+      <c r="L36" s="2"/>
+      <c r="M36" s="2"/>
+      <c r="N36" s="2"/>
+      <c r="O36" s="2"/>
+      <c r="P36" s="2"/>
+      <c r="Q36" s="2"/>
+      <c r="R36" s="2"/>
+      <c r="S36" s="2"/>
+      <c r="T36" s="2"/>
+      <c r="U36" s="2"/>
     </row>
     <row r="37" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="3"/>
-      <c r="B37" s="3"/>
-      <c r="C37" s="3"/>
-      <c r="D37" s="3"/>
-      <c r="E37" s="3"/>
-      <c r="F37" s="28"/>
-      <c r="G37" s="3"/>
-      <c r="H37" s="3"/>
-      <c r="I37" s="3"/>
-      <c r="J37" s="3"/>
-      <c r="K37" s="3"/>
-      <c r="L37" s="3"/>
-      <c r="M37" s="3"/>
-      <c r="N37" s="3"/>
-      <c r="O37" s="3"/>
-      <c r="P37" s="3"/>
-      <c r="Q37" s="3"/>
-      <c r="R37" s="3"/>
-      <c r="S37" s="3"/>
-      <c r="T37" s="3"/>
-      <c r="U37" s="3"/>
+      <c r="A37" s="2"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="17"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="2"/>
+      <c r="J37" s="2"/>
+      <c r="K37" s="2"/>
+      <c r="L37" s="2"/>
+      <c r="M37" s="2"/>
+      <c r="N37" s="2"/>
+      <c r="O37" s="2"/>
+      <c r="P37" s="2"/>
+      <c r="Q37" s="2"/>
+      <c r="R37" s="2"/>
+      <c r="S37" s="2"/>
+      <c r="T37" s="2"/>
+      <c r="U37" s="2"/>
     </row>
     <row r="38" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="3"/>
-      <c r="B38" s="3"/>
-      <c r="C38" s="3"/>
-      <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
-      <c r="F38" s="28"/>
-      <c r="G38" s="3"/>
-      <c r="H38" s="3"/>
-      <c r="I38" s="3"/>
-      <c r="J38" s="3"/>
-      <c r="K38" s="3"/>
-      <c r="L38" s="3"/>
-      <c r="M38" s="3"/>
-      <c r="N38" s="3"/>
-      <c r="O38" s="3"/>
-      <c r="P38" s="3"/>
-      <c r="Q38" s="3"/>
-      <c r="R38" s="3"/>
-      <c r="S38" s="3"/>
-      <c r="T38" s="3"/>
-      <c r="U38" s="3"/>
+      <c r="A38" s="2"/>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="17"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="2"/>
+      <c r="J38" s="2"/>
+      <c r="K38" s="2"/>
+      <c r="L38" s="2"/>
+      <c r="M38" s="2"/>
+      <c r="N38" s="2"/>
+      <c r="O38" s="2"/>
+      <c r="P38" s="2"/>
+      <c r="Q38" s="2"/>
+      <c r="R38" s="2"/>
+      <c r="S38" s="2"/>
+      <c r="T38" s="2"/>
+      <c r="U38" s="2"/>
     </row>
     <row r="39" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="3"/>
-      <c r="B39" s="3"/>
-      <c r="C39" s="3"/>
-      <c r="D39" s="3"/>
-      <c r="E39" s="3"/>
-      <c r="F39" s="28"/>
-      <c r="G39" s="3"/>
-      <c r="H39" s="3"/>
-      <c r="I39" s="3"/>
-      <c r="J39" s="3"/>
-      <c r="K39" s="3"/>
-      <c r="L39" s="3"/>
-      <c r="M39" s="3"/>
-      <c r="N39" s="3"/>
-      <c r="O39" s="3"/>
-      <c r="P39" s="3"/>
-      <c r="Q39" s="3"/>
-      <c r="R39" s="3"/>
-      <c r="S39" s="3"/>
-      <c r="T39" s="3"/>
-      <c r="U39" s="3"/>
+      <c r="A39" s="2"/>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="17"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="2"/>
+      <c r="J39" s="2"/>
+      <c r="K39" s="2"/>
+      <c r="L39" s="2"/>
+      <c r="M39" s="2"/>
+      <c r="N39" s="2"/>
+      <c r="O39" s="2"/>
+      <c r="P39" s="2"/>
+      <c r="Q39" s="2"/>
+      <c r="R39" s="2"/>
+      <c r="S39" s="2"/>
+      <c r="T39" s="2"/>
+      <c r="U39" s="2"/>
     </row>
     <row r="40" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="3"/>
-      <c r="B40" s="3"/>
-      <c r="C40" s="3"/>
-      <c r="D40" s="3"/>
-      <c r="E40" s="3"/>
-      <c r="F40" s="28"/>
-      <c r="G40" s="3"/>
-      <c r="H40" s="3"/>
-      <c r="I40" s="3"/>
-      <c r="J40" s="3"/>
-      <c r="K40" s="3"/>
-      <c r="L40" s="3"/>
-      <c r="M40" s="3"/>
-      <c r="N40" s="3"/>
-      <c r="O40" s="3"/>
-      <c r="P40" s="3"/>
-      <c r="Q40" s="3"/>
-      <c r="R40" s="3"/>
-      <c r="S40" s="3"/>
-      <c r="T40" s="3"/>
-      <c r="U40" s="3"/>
+      <c r="A40" s="2"/>
+      <c r="B40" s="2"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="17"/>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2"/>
+      <c r="I40" s="2"/>
+      <c r="J40" s="2"/>
+      <c r="K40" s="2"/>
+      <c r="L40" s="2"/>
+      <c r="M40" s="2"/>
+      <c r="N40" s="2"/>
+      <c r="O40" s="2"/>
+      <c r="P40" s="2"/>
+      <c r="Q40" s="2"/>
+      <c r="R40" s="2"/>
+      <c r="S40" s="2"/>
+      <c r="T40" s="2"/>
+      <c r="U40" s="2"/>
     </row>
     <row r="41" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="3"/>
-      <c r="B41" s="3"/>
-      <c r="C41" s="3"/>
-      <c r="D41" s="3"/>
-      <c r="E41" s="3"/>
-      <c r="F41" s="28"/>
-      <c r="G41" s="3"/>
-      <c r="H41" s="3"/>
-      <c r="I41" s="3"/>
-      <c r="J41" s="3"/>
-      <c r="K41" s="3"/>
-      <c r="L41" s="3"/>
-      <c r="M41" s="3"/>
-      <c r="N41" s="3"/>
-      <c r="O41" s="3"/>
-      <c r="P41" s="3"/>
-      <c r="Q41" s="3"/>
-      <c r="R41" s="3"/>
-      <c r="S41" s="3"/>
-      <c r="T41" s="3"/>
-      <c r="U41" s="3"/>
+      <c r="A41" s="2"/>
+      <c r="B41" s="2"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="17"/>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2"/>
+      <c r="I41" s="2"/>
+      <c r="J41" s="2"/>
+      <c r="K41" s="2"/>
+      <c r="L41" s="2"/>
+      <c r="M41" s="2"/>
+      <c r="N41" s="2"/>
+      <c r="O41" s="2"/>
+      <c r="P41" s="2"/>
+      <c r="Q41" s="2"/>
+      <c r="R41" s="2"/>
+      <c r="S41" s="2"/>
+      <c r="T41" s="2"/>
+      <c r="U41" s="2"/>
     </row>
     <row r="42" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="3"/>
-      <c r="B42" s="3"/>
-      <c r="C42" s="3"/>
-      <c r="D42" s="3"/>
-      <c r="E42" s="3"/>
-      <c r="F42" s="28"/>
-      <c r="G42" s="3"/>
-      <c r="H42" s="3"/>
-      <c r="I42" s="3"/>
-      <c r="J42" s="3"/>
-      <c r="K42" s="3"/>
-      <c r="L42" s="3"/>
-      <c r="M42" s="3"/>
-      <c r="N42" s="3"/>
-      <c r="O42" s="3"/>
-      <c r="P42" s="3"/>
-      <c r="Q42" s="3"/>
-      <c r="R42" s="3"/>
-      <c r="S42" s="3"/>
-      <c r="T42" s="3"/>
-      <c r="U42" s="3"/>
+      <c r="A42" s="2"/>
+      <c r="B42" s="2"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="17"/>
+      <c r="G42" s="2"/>
+      <c r="H42" s="2"/>
+      <c r="I42" s="2"/>
+      <c r="J42" s="2"/>
+      <c r="K42" s="2"/>
+      <c r="L42" s="2"/>
+      <c r="M42" s="2"/>
+      <c r="N42" s="2"/>
+      <c r="O42" s="2"/>
+      <c r="P42" s="2"/>
+      <c r="Q42" s="2"/>
+      <c r="R42" s="2"/>
+      <c r="S42" s="2"/>
+      <c r="T42" s="2"/>
+      <c r="U42" s="2"/>
     </row>
     <row r="43" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="3"/>
-      <c r="B43" s="3"/>
-      <c r="C43" s="3"/>
-      <c r="D43" s="3"/>
-      <c r="E43" s="3"/>
-      <c r="F43" s="28"/>
-      <c r="G43" s="3"/>
-      <c r="H43" s="3"/>
-      <c r="I43" s="3"/>
-      <c r="J43" s="3"/>
-      <c r="K43" s="3"/>
-      <c r="L43" s="3"/>
-      <c r="M43" s="3"/>
-      <c r="N43" s="3"/>
-      <c r="O43" s="3"/>
-      <c r="P43" s="3"/>
-      <c r="Q43" s="3"/>
-      <c r="R43" s="3"/>
-      <c r="S43" s="3"/>
-      <c r="T43" s="3"/>
-      <c r="U43" s="3"/>
+      <c r="A43" s="2"/>
+      <c r="B43" s="2"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="17"/>
+      <c r="G43" s="2"/>
+      <c r="H43" s="2"/>
+      <c r="I43" s="2"/>
+      <c r="J43" s="2"/>
+      <c r="K43" s="2"/>
+      <c r="L43" s="2"/>
+      <c r="M43" s="2"/>
+      <c r="N43" s="2"/>
+      <c r="O43" s="2"/>
+      <c r="P43" s="2"/>
+      <c r="Q43" s="2"/>
+      <c r="R43" s="2"/>
+      <c r="S43" s="2"/>
+      <c r="T43" s="2"/>
+      <c r="U43" s="2"/>
     </row>
     <row r="44" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="3"/>
-      <c r="B44" s="3"/>
-      <c r="C44" s="3"/>
-      <c r="D44" s="3"/>
-      <c r="E44" s="3"/>
-      <c r="F44" s="28"/>
-      <c r="G44" s="3"/>
-      <c r="H44" s="3"/>
-      <c r="I44" s="3"/>
-      <c r="J44" s="3"/>
-      <c r="K44" s="3"/>
-      <c r="L44" s="3"/>
-      <c r="M44" s="3"/>
-      <c r="N44" s="3"/>
-      <c r="O44" s="3"/>
-      <c r="P44" s="3"/>
-      <c r="Q44" s="3"/>
-      <c r="R44" s="3"/>
-      <c r="S44" s="3"/>
-      <c r="T44" s="3"/>
-      <c r="U44" s="3"/>
+      <c r="A44" s="2"/>
+      <c r="B44" s="2"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="17"/>
+      <c r="G44" s="2"/>
+      <c r="H44" s="2"/>
+      <c r="I44" s="2"/>
+      <c r="J44" s="2"/>
+      <c r="K44" s="2"/>
+      <c r="L44" s="2"/>
+      <c r="M44" s="2"/>
+      <c r="N44" s="2"/>
+      <c r="O44" s="2"/>
+      <c r="P44" s="2"/>
+      <c r="Q44" s="2"/>
+      <c r="R44" s="2"/>
+      <c r="S44" s="2"/>
+      <c r="T44" s="2"/>
+      <c r="U44" s="2"/>
     </row>
     <row r="45" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="3"/>
-      <c r="B45" s="3"/>
-      <c r="C45" s="3"/>
-      <c r="D45" s="3"/>
-      <c r="E45" s="3"/>
-      <c r="F45" s="28"/>
-      <c r="G45" s="3"/>
-      <c r="H45" s="3"/>
-      <c r="I45" s="3"/>
-      <c r="J45" s="3"/>
-      <c r="K45" s="3"/>
-      <c r="L45" s="3"/>
-      <c r="M45" s="3"/>
-      <c r="N45" s="3"/>
-      <c r="O45" s="3"/>
-      <c r="P45" s="3"/>
-      <c r="Q45" s="3"/>
-      <c r="R45" s="3"/>
-      <c r="S45" s="3"/>
-      <c r="T45" s="3"/>
-      <c r="U45" s="3"/>
+      <c r="A45" s="2"/>
+      <c r="B45" s="2"/>
+      <c r="C45" s="2"/>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="17"/>
+      <c r="G45" s="2"/>
+      <c r="H45" s="2"/>
+      <c r="I45" s="2"/>
+      <c r="J45" s="2"/>
+      <c r="K45" s="2"/>
+      <c r="L45" s="2"/>
+      <c r="M45" s="2"/>
+      <c r="N45" s="2"/>
+      <c r="O45" s="2"/>
+      <c r="P45" s="2"/>
+      <c r="Q45" s="2"/>
+      <c r="R45" s="2"/>
+      <c r="S45" s="2"/>
+      <c r="T45" s="2"/>
+      <c r="U45" s="2"/>
     </row>
     <row r="46" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="3"/>
-      <c r="B46" s="3"/>
-      <c r="C46" s="3"/>
-      <c r="D46" s="3"/>
-      <c r="E46" s="3"/>
-      <c r="F46" s="28"/>
-      <c r="G46" s="3"/>
-      <c r="H46" s="3"/>
-      <c r="I46" s="3"/>
-      <c r="J46" s="3"/>
-      <c r="K46" s="3"/>
-      <c r="L46" s="3"/>
-      <c r="M46" s="3"/>
-      <c r="N46" s="3"/>
-      <c r="O46" s="3"/>
-      <c r="P46" s="3"/>
-      <c r="Q46" s="3"/>
-      <c r="R46" s="3"/>
-      <c r="S46" s="3"/>
-      <c r="T46" s="3"/>
-      <c r="U46" s="3"/>
+      <c r="A46" s="2"/>
+      <c r="B46" s="2"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="17"/>
+      <c r="G46" s="2"/>
+      <c r="H46" s="2"/>
+      <c r="I46" s="2"/>
+      <c r="J46" s="2"/>
+      <c r="K46" s="2"/>
+      <c r="L46" s="2"/>
+      <c r="M46" s="2"/>
+      <c r="N46" s="2"/>
+      <c r="O46" s="2"/>
+      <c r="P46" s="2"/>
+      <c r="Q46" s="2"/>
+      <c r="R46" s="2"/>
+      <c r="S46" s="2"/>
+      <c r="T46" s="2"/>
+      <c r="U46" s="2"/>
     </row>
     <row r="47" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="3"/>
-      <c r="B47" s="3"/>
-      <c r="C47" s="3"/>
-      <c r="D47" s="3"/>
-      <c r="E47" s="3"/>
-      <c r="F47" s="28"/>
-      <c r="G47" s="3"/>
-      <c r="H47" s="3"/>
-      <c r="I47" s="3"/>
-      <c r="J47" s="3"/>
-      <c r="K47" s="3"/>
-      <c r="L47" s="3"/>
-      <c r="M47" s="3"/>
-      <c r="N47" s="3"/>
-      <c r="O47" s="3"/>
-      <c r="P47" s="3"/>
-      <c r="Q47" s="3"/>
-      <c r="R47" s="3"/>
-      <c r="S47" s="3"/>
-      <c r="T47" s="3"/>
-      <c r="U47" s="3"/>
+      <c r="A47" s="2"/>
+      <c r="B47" s="2"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
+      <c r="F47" s="17"/>
+      <c r="G47" s="2"/>
+      <c r="H47" s="2"/>
+      <c r="I47" s="2"/>
+      <c r="J47" s="2"/>
+      <c r="K47" s="2"/>
+      <c r="L47" s="2"/>
+      <c r="M47" s="2"/>
+      <c r="N47" s="2"/>
+      <c r="O47" s="2"/>
+      <c r="P47" s="2"/>
+      <c r="Q47" s="2"/>
+      <c r="R47" s="2"/>
+      <c r="S47" s="2"/>
+      <c r="T47" s="2"/>
+      <c r="U47" s="2"/>
     </row>
     <row r="48" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="3"/>
-      <c r="B48" s="3"/>
-      <c r="C48" s="3"/>
-      <c r="D48" s="3"/>
-      <c r="E48" s="3"/>
-      <c r="F48" s="28"/>
-      <c r="G48" s="3"/>
-      <c r="H48" s="3"/>
-      <c r="I48" s="3"/>
-      <c r="J48" s="3"/>
-      <c r="K48" s="3"/>
-      <c r="L48" s="3"/>
-      <c r="M48" s="3"/>
-      <c r="N48" s="3"/>
-      <c r="O48" s="3"/>
-      <c r="P48" s="3"/>
-      <c r="Q48" s="3"/>
-      <c r="R48" s="3"/>
-      <c r="S48" s="3"/>
-      <c r="T48" s="3"/>
-      <c r="U48" s="3"/>
+      <c r="A48" s="2"/>
+      <c r="B48" s="2"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
+      <c r="F48" s="17"/>
+      <c r="G48" s="2"/>
+      <c r="H48" s="2"/>
+      <c r="I48" s="2"/>
+      <c r="J48" s="2"/>
+      <c r="K48" s="2"/>
+      <c r="L48" s="2"/>
+      <c r="M48" s="2"/>
+      <c r="N48" s="2"/>
+      <c r="O48" s="2"/>
+      <c r="P48" s="2"/>
+      <c r="Q48" s="2"/>
+      <c r="R48" s="2"/>
+      <c r="S48" s="2"/>
+      <c r="T48" s="2"/>
+      <c r="U48" s="2"/>
     </row>
     <row r="49" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="3"/>
-      <c r="B49" s="3"/>
-      <c r="C49" s="3"/>
-      <c r="D49" s="3"/>
-      <c r="E49" s="3"/>
-      <c r="F49" s="28"/>
-      <c r="G49" s="3"/>
-      <c r="H49" s="3"/>
-      <c r="I49" s="3"/>
-      <c r="J49" s="3"/>
-      <c r="K49" s="3"/>
-      <c r="L49" s="3"/>
-      <c r="M49" s="3"/>
-      <c r="N49" s="3"/>
-      <c r="O49" s="3"/>
-      <c r="P49" s="3"/>
-      <c r="Q49" s="3"/>
-      <c r="R49" s="3"/>
-      <c r="S49" s="3"/>
-      <c r="T49" s="3"/>
-      <c r="U49" s="3"/>
+      <c r="A49" s="2"/>
+      <c r="B49" s="2"/>
+      <c r="C49" s="2"/>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
+      <c r="F49" s="17"/>
+      <c r="G49" s="2"/>
+      <c r="H49" s="2"/>
+      <c r="I49" s="2"/>
+      <c r="J49" s="2"/>
+      <c r="K49" s="2"/>
+      <c r="L49" s="2"/>
+      <c r="M49" s="2"/>
+      <c r="N49" s="2"/>
+      <c r="O49" s="2"/>
+      <c r="P49" s="2"/>
+      <c r="Q49" s="2"/>
+      <c r="R49" s="2"/>
+      <c r="S49" s="2"/>
+      <c r="T49" s="2"/>
+      <c r="U49" s="2"/>
     </row>
     <row r="50" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="3"/>
-      <c r="B50" s="3"/>
-      <c r="C50" s="3"/>
-      <c r="D50" s="3"/>
-      <c r="E50" s="3"/>
-      <c r="F50" s="28"/>
-      <c r="G50" s="3"/>
-      <c r="H50" s="3"/>
-      <c r="I50" s="3"/>
-      <c r="J50" s="3"/>
-      <c r="K50" s="3"/>
-      <c r="L50" s="3"/>
-      <c r="M50" s="3"/>
-      <c r="N50" s="3"/>
-      <c r="O50" s="3"/>
-      <c r="P50" s="3"/>
-      <c r="Q50" s="3"/>
-      <c r="R50" s="3"/>
-      <c r="S50" s="3"/>
-      <c r="T50" s="3"/>
-      <c r="U50" s="3"/>
-    </row>
-    <row r="51" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="3"/>
-      <c r="B51" s="3"/>
-      <c r="C51" s="3"/>
-      <c r="D51" s="3"/>
-      <c r="E51" s="3"/>
-      <c r="F51" s="28"/>
-      <c r="G51" s="3"/>
-      <c r="H51" s="3"/>
-      <c r="I51" s="3"/>
-      <c r="J51" s="3"/>
-      <c r="K51" s="3"/>
-      <c r="L51" s="3"/>
-      <c r="M51" s="3"/>
-      <c r="N51" s="3"/>
-      <c r="O51" s="3"/>
-      <c r="P51" s="3"/>
-      <c r="Q51" s="3"/>
-      <c r="R51" s="3"/>
-      <c r="S51" s="3"/>
-      <c r="T51" s="3"/>
-      <c r="U51" s="3"/>
+      <c r="A50" s="2"/>
+      <c r="B50" s="2"/>
+      <c r="C50" s="2"/>
+      <c r="D50" s="2"/>
+      <c r="E50" s="2"/>
+      <c r="F50" s="17"/>
+      <c r="G50" s="2"/>
+      <c r="H50" s="2"/>
+      <c r="I50" s="2"/>
+      <c r="J50" s="2"/>
+      <c r="K50" s="2"/>
+      <c r="L50" s="2"/>
+      <c r="M50" s="2"/>
+      <c r="N50" s="2"/>
+      <c r="O50" s="2"/>
+      <c r="P50" s="2"/>
+      <c r="Q50" s="2"/>
+      <c r="R50" s="2"/>
+      <c r="S50" s="2"/>
+      <c r="T50" s="2"/>
+      <c r="U50" s="2"/>
+    </row>
+    <row r="51" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="2"/>
+      <c r="B51" s="2"/>
+      <c r="C51" s="2"/>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
+      <c r="F51" s="17"/>
+      <c r="G51" s="2"/>
+      <c r="H51" s="2"/>
+      <c r="I51" s="2"/>
+      <c r="J51" s="2"/>
+      <c r="K51" s="2"/>
+      <c r="L51" s="2"/>
+      <c r="M51" s="2"/>
+      <c r="N51" s="2"/>
+      <c r="O51" s="2"/>
+      <c r="P51" s="2"/>
+      <c r="Q51" s="2"/>
+      <c r="R51" s="2"/>
+      <c r="S51" s="2"/>
+      <c r="T51" s="2"/>
+      <c r="U51" s="2"/>
     </row>
     <row r="52" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="3"/>
-      <c r="B52" s="3"/>
-      <c r="C52" s="3"/>
-      <c r="D52" s="3"/>
-      <c r="E52" s="3"/>
-      <c r="F52" s="28"/>
-      <c r="G52" s="3"/>
-      <c r="H52" s="3"/>
-      <c r="I52" s="3"/>
-      <c r="J52" s="3"/>
-      <c r="K52" s="3"/>
-      <c r="L52" s="3"/>
-      <c r="M52" s="3"/>
-      <c r="N52" s="3"/>
-      <c r="O52" s="3"/>
-      <c r="P52" s="3"/>
-      <c r="Q52" s="3"/>
-      <c r="R52" s="3"/>
-      <c r="S52" s="3"/>
-      <c r="T52" s="3"/>
-      <c r="U52" s="3"/>
-    </row>
-    <row r="53" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="A52" s="2"/>
+      <c r="B52" s="2"/>
+      <c r="C52" s="2"/>
+      <c r="D52" s="2"/>
+      <c r="E52" s="2"/>
+      <c r="F52" s="17"/>
+      <c r="G52" s="2"/>
+      <c r="H52" s="2"/>
+      <c r="I52" s="2"/>
+      <c r="J52" s="2"/>
+      <c r="K52" s="2"/>
+      <c r="L52" s="2"/>
+      <c r="M52" s="2"/>
+      <c r="N52" s="2"/>
+      <c r="O52" s="2"/>
+      <c r="P52" s="2"/>
+      <c r="Q52" s="2"/>
+      <c r="R52" s="2"/>
+      <c r="S52" s="2"/>
+      <c r="T52" s="2"/>
+      <c r="U52" s="2"/>
+    </row>
+    <row r="53" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="2"/>
+      <c r="B53" s="2"/>
+      <c r="C53" s="2"/>
+      <c r="D53" s="2"/>
+      <c r="E53" s="2"/>
+      <c r="F53" s="17"/>
+      <c r="G53" s="2"/>
+      <c r="H53" s="2"/>
+      <c r="I53" s="2"/>
+      <c r="J53" s="2"/>
+      <c r="K53" s="2"/>
+      <c r="L53" s="2"/>
+      <c r="M53" s="2"/>
+      <c r="N53" s="2"/>
+      <c r="O53" s="2"/>
+      <c r="P53" s="2"/>
+      <c r="Q53" s="2"/>
+      <c r="R53" s="2"/>
+      <c r="S53" s="2"/>
+      <c r="T53" s="2"/>
+      <c r="U53" s="2"/>
+    </row>
     <row r="54" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="55" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="56" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5670,6 +5717,7 @@
     <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A2:F2"/>
@@ -5705,13 +5753,13 @@
       <c r="B1" s="6"/>
     </row>
     <row r="2" spans="1:19" ht="37" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="25" t="s">
         <v>140</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
     </row>
     <row r="3" spans="1:19" ht="38" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
@@ -7741,13 +7789,13 @@
       <c r="B1" s="6"/>
     </row>
     <row r="2" spans="1:19" ht="37" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="25" t="s">
         <v>144</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
     </row>
     <row r="3" spans="1:19" ht="38" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
@@ -7767,19 +7815,19 @@
       </c>
     </row>
     <row r="4" spans="1:19" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="15">
+      <c r="A4" s="14">
         <v>45310</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="15" t="s">
         <v>151</v>
       </c>
-      <c r="C4" s="16" t="s">
-        <v>203</v>
-      </c>
-      <c r="D4" s="16" t="s">
+      <c r="C4" s="15" t="s">
+        <v>199</v>
+      </c>
+      <c r="D4" s="15" t="s">
         <v>152</v>
       </c>
-      <c r="E4" s="16" t="s">
+      <c r="E4" s="15" t="s">
         <v>153</v>
       </c>
       <c r="F4" s="2"/>
@@ -7798,19 +7846,19 @@
       <c r="S4" s="2"/>
     </row>
     <row r="5" spans="1:19" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="14">
+      <c r="A5" s="13">
         <v>45387</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>202</v>
-      </c>
-      <c r="C5" s="16" t="s">
-        <v>204</v>
-      </c>
-      <c r="D5" s="16" t="s">
+        <v>198</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>200</v>
+      </c>
+      <c r="D5" s="15" t="s">
         <v>152</v>
       </c>
-      <c r="E5" s="16" t="s">
+      <c r="E5" s="15" t="s">
         <v>153</v>
       </c>
       <c r="F5" s="2"/>

</xml_diff>

<commit_message>
add missing ISO codes for Tonga and Republic of Kiribati
</commit_message>
<xml_diff>
--- a/course-datasets/Data dictionary.xlsx
+++ b/course-datasets/Data dictionary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stepheaneff/Documents/work/GT/data-science-basics-2024/course-datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F69F291-8AE0-BE40-BAAA-1D55F7A50F42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDC5D7E0-1A19-5E4C-BBFB-5B56B5D53CAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="460" yWindow="760" windowWidth="29780" windowHeight="16820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="209">
   <si>
     <t>Text</t>
   </si>
@@ -514,6 +514,153 @@
   </si>
   <si>
     <t>one row per World Health Assembly member state</t>
+  </si>
+  <si>
+    <t>who_region</t>
+  </si>
+  <si>
+    <t>world_bank_region</t>
+  </si>
+  <si>
+    <t>income_group</t>
+  </si>
+  <si>
+    <t>total_population</t>
+  </si>
+  <si>
+    <t>pct_rural</t>
+  </si>
+  <si>
+    <t>measles_vaccine_policy</t>
+  </si>
+  <si>
+    <t>Region (WHO)</t>
+  </si>
+  <si>
+    <t>Region (World Bank)</t>
+  </si>
+  <si>
+    <t>Income group</t>
+  </si>
+  <si>
+    <t>Total population</t>
+  </si>
+  <si>
+    <t>Percent rural</t>
+  </si>
+  <si>
+    <t>Vaccine policy (measles)</t>
+  </si>
+  <si>
+    <t>measles_cases</t>
+  </si>
+  <si>
+    <t>measles_cases.tsv</t>
+  </si>
+  <si>
+    <t>one row per World Health Assembly member state per month</t>
+  </si>
+  <si>
+    <t>Country-level information, per month, on laboratory confirmed, epidemiologically linked, and/or clinical measles cases reported to the World Health Organization</t>
+  </si>
+  <si>
+    <t>World Health Organization. (22 March, 2024). Distribution of Measles Cases by Country and Month. https://www.who.int/teams/immunization-vaccines-and-biologicals/immunization-analysis-and-insights/surveillance/monitoring/provisional-monthly-measles-and-rubella-data</t>
+  </si>
+  <si>
+    <t>month</t>
+  </si>
+  <si>
+    <t>Month</t>
+  </si>
+  <si>
+    <t>Measles cases</t>
+  </si>
+  <si>
+    <t>Number of laboratory confirmed, epidemiologically linked, and/or clinical cases as reported to the World Health Organization by the country in the specified month</t>
+  </si>
+  <si>
+    <t>The ISO code of the country</t>
+  </si>
+  <si>
+    <t>character</t>
+  </si>
+  <si>
+    <t>ISO 3166 Country Codes. https://www.iso.org/iso-3166-country-codes.html</t>
+  </si>
+  <si>
+    <t>The name of the country</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>World Bank. (29 March, 2024). World Bank Country and Lending Groups. https://datahelpdesk.worldbank.org/knowledgebase/articles/906519-world-bank-country-and-lending-groups</t>
+  </si>
+  <si>
+    <t>World Health Organization. (20 February 2023). https://www.who.int/countries</t>
+  </si>
+  <si>
+    <t>The region of the country as designated by the World Health Organization (WHO), corresponding to the WHO regional office</t>
+  </si>
+  <si>
+    <t>The region of the country as designated by the World Bank</t>
+  </si>
+  <si>
+    <t>The income group of the country as designated by the World Bank for the year 2024</t>
+  </si>
+  <si>
+    <t>numeric</t>
+  </si>
+  <si>
+    <t>The total population of the country in the year 2024, as estimated by the World Bank</t>
+  </si>
+  <si>
+    <t>The percent of the total population living in a rural area, as estimated by the World Bank for the year 2024</t>
+  </si>
+  <si>
+    <t>Whether or not the country requires measles vaccination</t>
+  </si>
+  <si>
+    <t>The month for which data are reported</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>Completed initial data dictionary</t>
+  </si>
+  <si>
+    <t>Added initial notes</t>
+  </si>
+  <si>
+    <t>Updated data dictionary, though I anticipate more changes</t>
+  </si>
+  <si>
+    <t>Country-level information, including measles policy and vaccine coverage information, for World Health Assembly member states. Table also includes relevant information about the country including population size, region, and income designation</t>
+  </si>
+  <si>
+    <t>mcv1_coverage</t>
+  </si>
+  <si>
+    <t>Vaccine coverage (MCV1)</t>
+  </si>
+  <si>
+    <t>Internal GHSS research</t>
+  </si>
+  <si>
+    <t>World Health Organization. (5 April 2024). Measles-containing-vaccine first-dose (MCV1) immunization coverage among 1-year-olds (%). https://www.who.int/data/gho/data/indicators/indicator-details/GHO/measles-containing-vaccine-first-dose-(mcv1)-immunization-coverage-among-1-year-olds-(-)</t>
+  </si>
+  <si>
+    <t>countries.tsv</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The percentage of children under one year of age who have received at least one dose of measles-containing vaccine in a given year. For countries recommending the first dose of measles vaccine in children over 12 months of age, the indicator is calculated as the proportion of children less than 12-23 months of age receiving one dose of measles-containing vaccine. Data are the most recently reported to WHO and published as of April 2024.</t>
+  </si>
+  <si>
+    <t>World Health Organization. (10 February, 2023). Countries overview.  https://www.who.int/countries/ 
+World Bank. (29 March, 2024). World Bank Country and Lending Groups. https://datahelpdesk.worldbank.org/knowledgebase/articles/906519-world-bank-country-and-lending-groups
+World Bank. (29 March, 2024). Population estimates and projections, 2024. https://databank.worldbank.org/source/population-estimates-and-projections#
+Manually added missing ISO codes for Republic of Kiribati and Tonga</t>
   </si>
   <si>
     <r>
@@ -526,154 +673,11 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>April 5, 2024</t>
+      <t>May 22, 2024</t>
     </r>
   </si>
   <si>
-    <t>who_region</t>
-  </si>
-  <si>
-    <t>world_bank_region</t>
-  </si>
-  <si>
-    <t>income_group</t>
-  </si>
-  <si>
-    <t>total_population</t>
-  </si>
-  <si>
-    <t>pct_rural</t>
-  </si>
-  <si>
-    <t>measles_vaccine_policy</t>
-  </si>
-  <si>
-    <t>Region (WHO)</t>
-  </si>
-  <si>
-    <t>Region (World Bank)</t>
-  </si>
-  <si>
-    <t>Income group</t>
-  </si>
-  <si>
-    <t>Total population</t>
-  </si>
-  <si>
-    <t>Percent rural</t>
-  </si>
-  <si>
-    <t>Vaccine policy (measles)</t>
-  </si>
-  <si>
-    <t>measles_cases</t>
-  </si>
-  <si>
-    <t>measles_cases.tsv</t>
-  </si>
-  <si>
-    <t>one row per World Health Assembly member state per month</t>
-  </si>
-  <si>
-    <t>Country-level information, per month, on laboratory confirmed, epidemiologically linked, and/or clinical measles cases reported to the World Health Organization</t>
-  </si>
-  <si>
-    <t>World Health Organization. (10 February, 2023). Countries overview.  https://www.who.int/countries/ 
-World Bank. (29 March, 2024). World Bank Country and Lending Groups. https://datahelpdesk.worldbank.org/knowledgebase/articles/906519-world-bank-country-and-lending-groups
-World Bank. (29 March, 2024). Population estimates and projections, 2024. https://databank.worldbank.org/source/population-estimates-and-projections#</t>
-  </si>
-  <si>
-    <t>World Health Organization. (22 March, 2024). Distribution of Measles Cases by Country and Month. https://www.who.int/teams/immunization-vaccines-and-biologicals/immunization-analysis-and-insights/surveillance/monitoring/provisional-monthly-measles-and-rubella-data</t>
-  </si>
-  <si>
-    <t>month</t>
-  </si>
-  <si>
-    <t>Month</t>
-  </si>
-  <si>
-    <t>Measles cases</t>
-  </si>
-  <si>
-    <t>Number of laboratory confirmed, epidemiologically linked, and/or clinical cases as reported to the World Health Organization by the country in the specified month</t>
-  </si>
-  <si>
-    <t>The ISO code of the country</t>
-  </si>
-  <si>
-    <t>character</t>
-  </si>
-  <si>
-    <t>ISO 3166 Country Codes. https://www.iso.org/iso-3166-country-codes.html</t>
-  </si>
-  <si>
-    <t>The name of the country</t>
-  </si>
-  <si>
-    <t>N/A</t>
-  </si>
-  <si>
-    <t>World Bank. (29 March, 2024). World Bank Country and Lending Groups. https://datahelpdesk.worldbank.org/knowledgebase/articles/906519-world-bank-country-and-lending-groups</t>
-  </si>
-  <si>
-    <t>World Health Organization. (20 February 2023). https://www.who.int/countries</t>
-  </si>
-  <si>
-    <t>The region of the country as designated by the World Health Organization (WHO), corresponding to the WHO regional office</t>
-  </si>
-  <si>
-    <t>The region of the country as designated by the World Bank</t>
-  </si>
-  <si>
-    <t>The income group of the country as designated by the World Bank for the year 2024</t>
-  </si>
-  <si>
-    <t>numeric</t>
-  </si>
-  <si>
-    <t>The total population of the country in the year 2024, as estimated by the World Bank</t>
-  </si>
-  <si>
-    <t>The percent of the total population living in a rural area, as estimated by the World Bank for the year 2024</t>
-  </si>
-  <si>
-    <t>Whether or not the country requires measles vaccination</t>
-  </si>
-  <si>
-    <t>The month for which data are reported</t>
-  </si>
-  <si>
-    <t>date</t>
-  </si>
-  <si>
-    <t>Completed initial data dictionary</t>
-  </si>
-  <si>
-    <t>Added initial notes</t>
-  </si>
-  <si>
-    <t>Updated data dictionary, though I anticipate more changes</t>
-  </si>
-  <si>
-    <t>Country-level information, including measles policy and vaccine coverage information, for World Health Assembly member states. Table also includes relevant information about the country including population size, region, and income designation</t>
-  </si>
-  <si>
-    <t>mcv1_coverage</t>
-  </si>
-  <si>
-    <t>Vaccine coverage (MCV1)</t>
-  </si>
-  <si>
-    <t>Internal GHSS research</t>
-  </si>
-  <si>
-    <t>World Health Organization. (5 April 2024). Measles-containing-vaccine first-dose (MCV1) immunization coverage among 1-year-olds (%). https://www.who.int/data/gho/data/indicators/indicator-details/GHO/measles-containing-vaccine-first-dose-(mcv1)-immunization-coverage-among-1-year-olds-(-)</t>
-  </si>
-  <si>
-    <t>countries.tsv</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> The percentage of children under one year of age who have received at least one dose of measles-containing vaccine in a given year. For countries recommending the first dose of measles vaccine in children over 12 months of age, the indicator is calculated as the proportion of children less than 12-23 months of age receiving one dose of measles-containing vaccine. Data are the most recently reported to WHO and published as of April 2024.</t>
+    <t>ISO 3166 Country Codes. https://www.iso.org/iso-3166-country-codes.html // Manually added missing ISO codes for Republic of Kiribati and Tonga</t>
   </si>
 </sst>
 </file>
@@ -1172,7 +1176,7 @@
   <dimension ref="A1:V1003"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1201,7 +1205,7 @@
     </row>
     <row r="3" spans="1:22" ht="17" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="24" t="s">
-        <v>159</v>
+        <v>207</v>
       </c>
       <c r="B3" s="24"/>
       <c r="C3" s="24"/>
@@ -1248,12 +1252,12 @@
         <v>143</v>
       </c>
     </row>
-    <row r="8" spans="1:22" ht="152" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:22" ht="166" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C8" s="10" t="s">
         <v>158</v>
@@ -1262,7 +1266,7 @@
         <v>149</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>176</v>
+        <v>206</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -1284,19 +1288,19 @@
     </row>
     <row r="9" spans="1:22" ht="100" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="C9" s="8" t="s">
         <v>173</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>175</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>174</v>
       </c>
       <c r="D9" s="9" t="s">
         <v>149</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -3414,8 +3418,8 @@
   </sheetPr>
   <dimension ref="A1:U1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3467,7 +3471,7 @@
     </row>
     <row r="4" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>155</v>
@@ -3476,13 +3480,13 @@
         <v>157</v>
       </c>
       <c r="D4" s="19" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E4" s="20" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="F4" s="20" t="s">
-        <v>184</v>
+        <v>208</v>
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
@@ -3502,7 +3506,7 @@
     </row>
     <row r="5" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>154</v>
@@ -3511,13 +3515,13 @@
         <v>156</v>
       </c>
       <c r="D5" s="19" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="F5" s="20" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
@@ -3537,22 +3541,22 @@
     </row>
     <row r="6" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="F6" s="20" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
@@ -3572,22 +3576,22 @@
     </row>
     <row r="7" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="F7" s="20" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
@@ -3607,22 +3611,22 @@
     </row>
     <row r="8" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E8" s="20" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="F8" s="20" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
@@ -3642,22 +3646,22 @@
     </row>
     <row r="9" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D9" s="19" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E9" s="20" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F9" s="20" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
@@ -3677,22 +3681,22 @@
     </row>
     <row r="10" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E10" s="20" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F10" s="20" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
@@ -3712,22 +3716,22 @@
     </row>
     <row r="11" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E11" s="20" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F11" s="20" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
@@ -3747,22 +3751,22 @@
     </row>
     <row r="12" spans="1:21" ht="141" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C12" s="8" t="s">
+        <v>201</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>205</v>
+      </c>
+      <c r="E12" s="20" t="s">
+        <v>190</v>
+      </c>
+      <c r="F12" s="20" t="s">
         <v>203</v>
-      </c>
-      <c r="D12" s="19" t="s">
-        <v>207</v>
-      </c>
-      <c r="E12" s="20" t="s">
-        <v>192</v>
-      </c>
-      <c r="F12" s="20" t="s">
-        <v>205</v>
       </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
@@ -3782,7 +3786,7 @@
     </row>
     <row r="13" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B13" s="8" t="s">
         <v>155</v>
@@ -3791,13 +3795,13 @@
         <v>157</v>
       </c>
       <c r="D13" s="19" t="s">
+        <v>180</v>
+      </c>
+      <c r="E13" s="20" t="s">
+        <v>181</v>
+      </c>
+      <c r="F13" s="20" t="s">
         <v>182</v>
-      </c>
-      <c r="E13" s="20" t="s">
-        <v>183</v>
-      </c>
-      <c r="F13" s="20" t="s">
-        <v>184</v>
       </c>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
@@ -3817,7 +3821,7 @@
     </row>
     <row r="14" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B14" s="8" t="s">
         <v>154</v>
@@ -3826,13 +3830,13 @@
         <v>156</v>
       </c>
       <c r="D14" s="19" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E14" s="20" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="F14" s="20" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
@@ -3852,22 +3856,22 @@
     </row>
     <row r="15" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E15" s="20" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F15" s="16" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
@@ -3887,22 +3891,22 @@
     </row>
     <row r="16" spans="1:21" ht="70" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E16" s="20" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F16" s="16" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
@@ -7822,7 +7826,7 @@
         <v>151</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D4" s="15" t="s">
         <v>152</v>
@@ -7850,10 +7854,10 @@
         <v>45387</v>
       </c>
       <c r="B5" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="C5" s="15" t="s">
         <v>198</v>
-      </c>
-      <c r="C5" s="15" t="s">
-        <v>200</v>
       </c>
       <c r="D5" s="15" t="s">
         <v>152</v>

</xml_diff>

<commit_message>
add income and region information to measles caseload dataset
</commit_message>
<xml_diff>
--- a/course-datasets/Data dictionary.xlsx
+++ b/course-datasets/Data dictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stepheaneff/Documents/work/GT/data-science-basics-2024/course-datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDC5D7E0-1A19-5E4C-BBFB-5B56B5D53CAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FB4AD17-BD68-7A42-BCC5-5985863263C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="460" yWindow="760" windowWidth="29780" windowHeight="16820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2940" yWindow="880" windowWidth="29780" windowHeight="16820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table information" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="213">
   <si>
     <t>Text</t>
   </si>
@@ -678,6 +678,18 @@
   </si>
   <si>
     <t>ISO 3166 Country Codes. https://www.iso.org/iso-3166-country-codes.html // Manually added missing ISO codes for Republic of Kiribati and Tonga</t>
+  </si>
+  <si>
+    <t>WHO region</t>
+  </si>
+  <si>
+    <t>World Bank region</t>
+  </si>
+  <si>
+    <t>Added additional fields to measles_cases dataset</t>
+  </si>
+  <si>
+    <t>Ongoing updates</t>
   </si>
 </sst>
 </file>
@@ -1176,7 +1188,7 @@
   <dimension ref="A1:V1003"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="A2" sqref="A2:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3418,8 +3430,8 @@
   </sheetPr>
   <dimension ref="A1:U1000"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17:F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3925,12 +3937,24 @@
       <c r="U16" s="2"/>
     </row>
     <row r="17" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="17"/>
+      <c r="A17" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="D17" s="19" t="s">
+        <v>187</v>
+      </c>
+      <c r="E17" s="20" t="s">
+        <v>181</v>
+      </c>
+      <c r="F17" s="20" t="s">
+        <v>186</v>
+      </c>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
@@ -3948,12 +3972,24 @@
       <c r="U17" s="2"/>
     </row>
     <row r="18" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="17"/>
+      <c r="A18" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="D18" s="19" t="s">
+        <v>188</v>
+      </c>
+      <c r="E18" s="20" t="s">
+        <v>181</v>
+      </c>
+      <c r="F18" s="20" t="s">
+        <v>185</v>
+      </c>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
@@ -3971,12 +4007,24 @@
       <c r="U18" s="2"/>
     </row>
     <row r="19" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="17"/>
+      <c r="A19" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="D19" s="19" t="s">
+        <v>189</v>
+      </c>
+      <c r="E19" s="20" t="s">
+        <v>181</v>
+      </c>
+      <c r="F19" s="20" t="s">
+        <v>185</v>
+      </c>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
@@ -7776,7 +7824,7 @@
   <dimension ref="A1:S997"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -7881,10 +7929,18 @@
       <c r="S5" s="2"/>
     </row>
     <row r="6" spans="1:19" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="7"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
+      <c r="A6" s="13">
+        <v>45434</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>212</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>152</v>
+      </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>

</xml_diff>

<commit_message>
add income group for Venezuela
</commit_message>
<xml_diff>
--- a/course-datasets/Data dictionary.xlsx
+++ b/course-datasets/Data dictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stepheaneff/Documents/work/GT/data-science-basics-2024/course-datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEF4F585-3E66-CB42-A20C-8D0F0A452600}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56FEF8C3-0ED2-4044-B114-88F071D1EFD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="640" yWindow="760" windowWidth="29780" windowHeight="16820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="460" yWindow="760" windowWidth="29780" windowHeight="16820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table information" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="276">
   <si>
     <t>Text</t>
   </si>
@@ -876,6 +876,9 @@
   </si>
   <si>
     <t>Measles-containing-vaccine first-dose (MCV1) immunization coverage among 1-year-olds, as a percentage</t>
+  </si>
+  <si>
+    <t>World Bank. (29 March, 2024). World Bank Country and Lending Groups. https://datahelpdesk.worldbank.org/knowledgebase/articles/906519-world-bank-country-and-lending-groups. Data for Venezuela missing from this data source and manually added to input dataset based on information from https://publicadministration.un.org/egovkb/en-us/Data/Country-Information/id/188-Venezuela as of May 24, 2024</t>
   </si>
 </sst>
 </file>
@@ -3703,8 +3706,8 @@
   </sheetPr>
   <dimension ref="A1:U1008"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3911,7 +3914,7 @@
         <v>181</v>
       </c>
       <c r="F8" s="18" t="s">
-        <v>185</v>
+        <v>275</v>
       </c>
       <c r="G8" s="26"/>
       <c r="H8" s="26"/>

</xml_diff>

<commit_message>
initial commit of energy dataset
</commit_message>
<xml_diff>
--- a/course-datasets/Data dictionary.xlsx
+++ b/course-datasets/Data dictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stepheaneff/Documents/work/GT/data-science-basics-2024/course-datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56FEF8C3-0ED2-4044-B114-88F071D1EFD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{329C92E2-32E4-004B-8097-65CCAA30DC3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="460" yWindow="760" windowWidth="29780" windowHeight="16820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="460" yWindow="760" windowWidth="29780" windowHeight="16820" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table information" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="738" uniqueCount="410">
   <si>
     <t>Text</t>
   </si>
@@ -879,6 +879,408 @@
   </si>
   <si>
     <t>World Bank. (29 March, 2024). World Bank Country and Lending Groups. https://datahelpdesk.worldbank.org/knowledgebase/articles/906519-world-bank-country-and-lending-groups. Data for Venezuela missing from this data source and manually added to input dataset based on information from https://publicadministration.un.org/egovkb/en-us/Data/Country-Information/id/188-Venezuela as of May 24, 2024</t>
+  </si>
+  <si>
+    <t>energy_2022.tsv</t>
+  </si>
+  <si>
+    <t>Country-level information related to energy supply and utilization, as of the year 2022</t>
+  </si>
+  <si>
+    <t>one row per country</t>
+  </si>
+  <si>
+    <t>Hannah Ritchie, Pablo Rosado and Max Roser (2023). “Energy”, OurWorldInData.org.  'https://ourworldindata.org/energy'</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>population</t>
+  </si>
+  <si>
+    <t>gdp</t>
+  </si>
+  <si>
+    <t>biofuel_elec_per_capita</t>
+  </si>
+  <si>
+    <t>biofuel_electricity</t>
+  </si>
+  <si>
+    <t>biofuel_share_elec</t>
+  </si>
+  <si>
+    <t>carbon_intensity_elec</t>
+  </si>
+  <si>
+    <t>coal_elec_per_capita</t>
+  </si>
+  <si>
+    <t>coal_electricity</t>
+  </si>
+  <si>
+    <t>coal_share_elec</t>
+  </si>
+  <si>
+    <t>electricity_demand</t>
+  </si>
+  <si>
+    <t>electricity_generation</t>
+  </si>
+  <si>
+    <t>fossil_elec_per_capita</t>
+  </si>
+  <si>
+    <t>fossil_electricity</t>
+  </si>
+  <si>
+    <t>fossil_share_elec</t>
+  </si>
+  <si>
+    <t>gas_elec_per_capita</t>
+  </si>
+  <si>
+    <t>gas_electricity</t>
+  </si>
+  <si>
+    <t>gas_share_elec</t>
+  </si>
+  <si>
+    <t>greenhouse_gas_emissions</t>
+  </si>
+  <si>
+    <t>hydro_elec_per_capita</t>
+  </si>
+  <si>
+    <t>hydro_electricity</t>
+  </si>
+  <si>
+    <t>hydro_share_elec</t>
+  </si>
+  <si>
+    <t>low_carbon_elec_per_capita</t>
+  </si>
+  <si>
+    <t>low_carbon_electricity</t>
+  </si>
+  <si>
+    <t>low_carbon_share_elec</t>
+  </si>
+  <si>
+    <t>net_elec_imports</t>
+  </si>
+  <si>
+    <t>net_elec_imports_share_demand</t>
+  </si>
+  <si>
+    <t>nuclear_elec_per_capita</t>
+  </si>
+  <si>
+    <t>nuclear_electricity</t>
+  </si>
+  <si>
+    <t>nuclear_share_elec</t>
+  </si>
+  <si>
+    <t>oil_elec_per_capita</t>
+  </si>
+  <si>
+    <t>oil_electricity</t>
+  </si>
+  <si>
+    <t>oil_share_elec</t>
+  </si>
+  <si>
+    <t>other_renewable_electricity</t>
+  </si>
+  <si>
+    <t>other_renewables_elec_per_capita</t>
+  </si>
+  <si>
+    <t>per_capita_electricity</t>
+  </si>
+  <si>
+    <t>renewables_elec_per_capita</t>
+  </si>
+  <si>
+    <t>renewables_electricity</t>
+  </si>
+  <si>
+    <t>renewables_share_elec</t>
+  </si>
+  <si>
+    <t>solar_electricity</t>
+  </si>
+  <si>
+    <t>solar_share_elec</t>
+  </si>
+  <si>
+    <t>wind_elec_per_capita</t>
+  </si>
+  <si>
+    <t>wind_electricity</t>
+  </si>
+  <si>
+    <t>wind_share_elec</t>
+  </si>
+  <si>
+    <t>Country population</t>
+  </si>
+  <si>
+    <t>Population - Population by country, available from 10,000 BCE to 2100, based on data and estimates from different sources.</t>
+  </si>
+  <si>
+    <t>Gross domestic product (GDP) - This data is adjusted for inflation and differences in the cost of living between countries.</t>
+  </si>
+  <si>
+    <t>Electricity generation from bioenergy per person - Measured in kilowatt-hours per person.</t>
+  </si>
+  <si>
+    <t>Electricity generation from bioenergy - Measured in terawatt-hours.</t>
+  </si>
+  <si>
+    <t>Share of electricity generated by bioenergy - Measured as a percentage of total electricity.</t>
+  </si>
+  <si>
+    <t>Carbon intensity of electricity generation - Greenhouse gases emitted per unit of generated electricity, measured in grams of CO₂ equivalents per kilowatt-hour.</t>
+  </si>
+  <si>
+    <t>Electricity generation from coal per person - Measured in kilowatt-hours per person.</t>
+  </si>
+  <si>
+    <t>Electricity generation from coal - Measured in terawatt-hours.</t>
+  </si>
+  <si>
+    <t>Share of electricity generated by coal - Measured as a percentage of total electricity.</t>
+  </si>
+  <si>
+    <t>Electricity demand - Measured in terawatt-hours.</t>
+  </si>
+  <si>
+    <t>Total electricity generation - Measured in terawatt-hours.</t>
+  </si>
+  <si>
+    <t>Fossil fuel consumption per capita - Measured in kilowatt-hours per person.</t>
+  </si>
+  <si>
+    <t>Electricity generation from fossil fuels - Measured in terawatt-hours.</t>
+  </si>
+  <si>
+    <t>Share of electricity generated by fossil fuels - Measured as a percentage of total electricity.</t>
+  </si>
+  <si>
+    <t>Gas consumption per capita - Measured in kilowatt-hours per person.</t>
+  </si>
+  <si>
+    <t>Electricity generation from gas - Measured in terawatt-hours.</t>
+  </si>
+  <si>
+    <t>Share of electricity generated by gas - Measured as a percentage of total electricity.</t>
+  </si>
+  <si>
+    <t>Emissions from electricity generation - Measured in megatonnes of CO₂ equivalents.</t>
+  </si>
+  <si>
+    <t>Electricity generation from hydropower per person - Measured in kilowatt-hours per person.</t>
+  </si>
+  <si>
+    <t>Electricity generation from hydropower - Measured in terawatt-hours.</t>
+  </si>
+  <si>
+    <t>Share of electricity generated by hydropower - Measured as a percentage of total electricity.</t>
+  </si>
+  <si>
+    <t>Low-carbon energy consumption per capita - Measured in kilowatt-hours per person.</t>
+  </si>
+  <si>
+    <t>Electricity generation from low-carbon sources - Low-carbon sources correspond to renewables and nuclear power, that produce significantly less greenhouse-gas emissions than fossil fuels.</t>
+  </si>
+  <si>
+    <t>Share of electricity generated by low-carbon sources - Low-carbon sources correspond to renewables and nuclear power, that produce significantly less greenhouse-gas emissions than fossil fuels.</t>
+  </si>
+  <si>
+    <t>Net electricity imports - Electricity imports minus exports, measured in TWh.</t>
+  </si>
+  <si>
+    <t>Net electricity imports as a share of demand - Electricity imports minus exports, measured as a percentage of total electricity demand.</t>
+  </si>
+  <si>
+    <t>Electricity generation from nuclear power per person - Measured in kilowatt-hours per person.</t>
+  </si>
+  <si>
+    <t>Electricity generation from nuclear - Measured in terawatt-hours.</t>
+  </si>
+  <si>
+    <t>Share of electricity generated by nuclear power - Measured as a percentage of total electricity.</t>
+  </si>
+  <si>
+    <t>Electricity generation from oil per person - Measured in kilowatt-hours per person.</t>
+  </si>
+  <si>
+    <t>Electricity generation from oil - Measured in terawatt-hours.</t>
+  </si>
+  <si>
+    <t>Share of electricity generated by oil - Measured as a percentage of total electricity.</t>
+  </si>
+  <si>
+    <t>Electricity generation from other renewables, including bioenergy - Measured in terawatt-hours.</t>
+  </si>
+  <si>
+    <t>Electricity generation from other renewables, including bioenergy, per person - Measured in kilowatt-hours per person.</t>
+  </si>
+  <si>
+    <t>Total electricity generation per person - Measured in kilowatt-hours per person.</t>
+  </si>
+  <si>
+    <t>Electricity generation from renewables per person - Measured in kilowatt-hours per person.</t>
+  </si>
+  <si>
+    <t>Electricity generation from renewables - Measured in terawatt-hours.</t>
+  </si>
+  <si>
+    <t>Share of electricity generated by renewables - Measured as a percentage of total electricity.</t>
+  </si>
+  <si>
+    <t>Electricity generation from solar power - Measured in terawatt-hours.</t>
+  </si>
+  <si>
+    <t>Share of electricity generated by solar power - Measured as a percentage of total electricity.</t>
+  </si>
+  <si>
+    <t>Electricity generation from wind power per person - Measured in kilowatt-hours per person.</t>
+  </si>
+  <si>
+    <t>Electricity generation from wind power - Measured in terawatt-hours.</t>
+  </si>
+  <si>
+    <t>Share of electricity generated by wind power - Measured as a percentage of total electricity.</t>
+  </si>
+  <si>
+    <t>GDP</t>
+  </si>
+  <si>
+    <t>Electricity generation from bioenergy per person</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Electricity generation from bioenergy </t>
+  </si>
+  <si>
+    <t>Share of electricity generated by bioenergy</t>
+  </si>
+  <si>
+    <t>Carbon intensity of electricity generation</t>
+  </si>
+  <si>
+    <t>Electricity generation from coal per person</t>
+  </si>
+  <si>
+    <t>Electricity generation from coal</t>
+  </si>
+  <si>
+    <t>Share of electricity generated by coal</t>
+  </si>
+  <si>
+    <t>Electricity demand</t>
+  </si>
+  <si>
+    <t>Total electricity generation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fossil fuel consumption per capita </t>
+  </si>
+  <si>
+    <t>Electricity generation from fossil fuels</t>
+  </si>
+  <si>
+    <t>Share of electricity generated by fossil fuels</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gas consumption per capita </t>
+  </si>
+  <si>
+    <t>Electricity generation from gas</t>
+  </si>
+  <si>
+    <t>Share of electricity generated by gas</t>
+  </si>
+  <si>
+    <t>Emissions from electricity generation</t>
+  </si>
+  <si>
+    <t>Electricity generation from hydropower per person</t>
+  </si>
+  <si>
+    <t>Electricity generation from hydropower</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Share of electricity generated by hydropower </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Low-carbon energy consumption per capita </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Electricity generation from low-carbon sources </t>
+  </si>
+  <si>
+    <t>Share of electricity generated by low-carbon sources</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Net electricity imports </t>
+  </si>
+  <si>
+    <t>Net electricity imports as a share of demand</t>
+  </si>
+  <si>
+    <t>Electricity generation from nuclear power per person</t>
+  </si>
+  <si>
+    <t>Electricity generation from nuclear</t>
+  </si>
+  <si>
+    <t>Share of electricity generated by nuclear power</t>
+  </si>
+  <si>
+    <t>Electricity generation from oil per person</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Electricity generation from oil </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Share of electricity generated by oil </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Electricity generation from other renewables, including bioenergy </t>
+  </si>
+  <si>
+    <t>Electricity generation from other renewables, including bioenergy, per person</t>
+  </si>
+  <si>
+    <t>Total electricity generation per person</t>
+  </si>
+  <si>
+    <t>Electricity generation from renewables per person</t>
+  </si>
+  <si>
+    <t>Electricity generation from renewables</t>
+  </si>
+  <si>
+    <t>Share of electricity generated by renewables</t>
+  </si>
+  <si>
+    <t>Electricity generation from solar power</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Share of electricity generated by solar power </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Electricity generation from wind power per person </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Electricity generation from wind power </t>
+  </si>
+  <si>
+    <t>Share of electricity generated by wind power</t>
   </si>
 </sst>
 </file>
@@ -1032,7 +1434,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1111,9 +1513,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1132,6 +1531,8 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1407,10 +1808,10 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:V1004"/>
+  <dimension ref="A1:V1005"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:E6"/>
+    <sheetView topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1423,51 +1824,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="124" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="29"/>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
+      <c r="A1" s="28"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
     </row>
     <row r="2" spans="1:22" ht="17" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="29" t="s">
         <v>150</v>
       </c>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
     </row>
     <row r="3" spans="1:22" ht="17" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="30" t="s">
         <v>264</v>
       </c>
-      <c r="B3" s="31"/>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
     </row>
     <row r="4" spans="1:22" ht="17" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="30" t="s">
         <v>148</v>
       </c>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
     </row>
     <row r="5" spans="1:22" ht="17" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
-      <c r="B5" s="33"/>
-      <c r="C5" s="33"/>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
+      <c r="B5" s="32"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
     </row>
     <row r="6" spans="1:22" ht="37" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A6" s="32" t="s">
+      <c r="A6" s="31" t="s">
         <v>132</v>
       </c>
-      <c r="B6" s="32"/>
-      <c r="C6" s="32"/>
-      <c r="D6" s="32"/>
-      <c r="E6" s="32"/>
+      <c r="B6" s="31"/>
+      <c r="C6" s="31"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="31"/>
     </row>
     <row r="7" spans="1:22" ht="32.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
@@ -1588,21 +1989,21 @@
       <c r="U10" s="2"/>
       <c r="V10" s="2"/>
     </row>
-    <row r="11" spans="1:22" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:22" ht="100" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
-        <v>212</v>
+        <v>276</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>213</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>214</v>
+        <v>277</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>278</v>
       </c>
       <c r="D11" s="9" t="s">
         <v>149</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>215</v>
+        <v>279</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
@@ -1624,13 +2025,13 @@
     </row>
     <row r="12" spans="1:22" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
-        <v>239</v>
+        <v>212</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>241</v>
+        <v>213</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>240</v>
+        <v>214</v>
       </c>
       <c r="D12" s="9" t="s">
         <v>149</v>
@@ -1657,11 +2058,21 @@
       <c r="V12" s="2"/>
     </row>
     <row r="13" spans="1:22" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="7"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="2"/>
+      <c r="A13" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>241</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>240</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>215</v>
+      </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
@@ -1683,7 +2094,7 @@
     <row r="14" spans="1:22" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="7"/>
       <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
+      <c r="C14" s="9"/>
       <c r="D14" s="9"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
@@ -1705,10 +2116,10 @@
       <c r="V14" s="2"/>
     </row>
     <row r="15" spans="1:22" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
+      <c r="A15" s="7"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="9"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
@@ -1753,8 +2164,8 @@
       <c r="V16" s="2"/>
     </row>
     <row r="17" spans="1:22" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
@@ -2233,28 +2644,28 @@
       <c r="V36" s="2"/>
     </row>
     <row r="37" spans="1:22" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="3"/>
-      <c r="B37" s="3"/>
-      <c r="C37" s="3"/>
-      <c r="D37" s="3"/>
-      <c r="E37" s="3"/>
-      <c r="F37" s="3"/>
-      <c r="G37" s="3"/>
-      <c r="H37" s="3"/>
-      <c r="I37" s="3"/>
-      <c r="J37" s="3"/>
-      <c r="K37" s="3"/>
-      <c r="L37" s="3"/>
-      <c r="M37" s="3"/>
-      <c r="N37" s="3"/>
-      <c r="O37" s="3"/>
-      <c r="P37" s="3"/>
-      <c r="Q37" s="3"/>
-      <c r="R37" s="3"/>
-      <c r="S37" s="3"/>
-      <c r="T37" s="3"/>
-      <c r="U37" s="3"/>
-      <c r="V37" s="3"/>
+      <c r="A37" s="2"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="2"/>
+      <c r="J37" s="2"/>
+      <c r="K37" s="2"/>
+      <c r="L37" s="2"/>
+      <c r="M37" s="2"/>
+      <c r="N37" s="2"/>
+      <c r="O37" s="2"/>
+      <c r="P37" s="2"/>
+      <c r="Q37" s="2"/>
+      <c r="R37" s="2"/>
+      <c r="S37" s="2"/>
+      <c r="T37" s="2"/>
+      <c r="U37" s="2"/>
+      <c r="V37" s="2"/>
     </row>
     <row r="38" spans="1:22" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="3"/>
@@ -2592,7 +3003,7 @@
       <c r="U51" s="3"/>
       <c r="V51" s="3"/>
     </row>
-    <row r="52" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:22" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="3"/>
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
@@ -2736,7 +3147,30 @@
       <c r="U57" s="3"/>
       <c r="V57" s="3"/>
     </row>
-    <row r="58" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="58" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="3"/>
+      <c r="B58" s="3"/>
+      <c r="C58" s="3"/>
+      <c r="D58" s="3"/>
+      <c r="E58" s="3"/>
+      <c r="F58" s="3"/>
+      <c r="G58" s="3"/>
+      <c r="H58" s="3"/>
+      <c r="I58" s="3"/>
+      <c r="J58" s="3"/>
+      <c r="K58" s="3"/>
+      <c r="L58" s="3"/>
+      <c r="M58" s="3"/>
+      <c r="N58" s="3"/>
+      <c r="O58" s="3"/>
+      <c r="P58" s="3"/>
+      <c r="Q58" s="3"/>
+      <c r="R58" s="3"/>
+      <c r="S58" s="3"/>
+      <c r="T58" s="3"/>
+      <c r="U58" s="3"/>
+      <c r="V58" s="3"/>
+    </row>
     <row r="59" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="60" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="61" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3683,6 +4117,7 @@
     <row r="1002" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1003" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1004" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1005" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="A1:E1"/>
@@ -3704,10 +4139,10 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:U1008"/>
+  <dimension ref="A1:U1048576"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E51" sqref="E51:E88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3728,14 +4163,14 @@
       <c r="D1" s="20"/>
     </row>
     <row r="2" spans="1:21" ht="37" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="33" t="s">
         <v>137</v>
       </c>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
     </row>
     <row r="3" spans="1:21" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A3" s="24" t="s">
@@ -5159,13 +5594,25 @@
       <c r="T43" s="26"/>
       <c r="U43" s="26"/>
     </row>
-    <row r="44" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="26"/>
-      <c r="B44" s="26"/>
-      <c r="C44" s="26"/>
-      <c r="D44" s="26"/>
-      <c r="E44" s="26"/>
-      <c r="F44" s="28"/>
+    <row r="44" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="B44" s="34" t="s">
+        <v>280</v>
+      </c>
+      <c r="C44" s="21" t="s">
+        <v>216</v>
+      </c>
+      <c r="D44" s="21" t="s">
+        <v>183</v>
+      </c>
+      <c r="E44" s="21" t="s">
+        <v>181</v>
+      </c>
+      <c r="F44" s="9" t="s">
+        <v>279</v>
+      </c>
       <c r="G44" s="26"/>
       <c r="H44" s="26"/>
       <c r="I44" s="26"/>
@@ -5182,13 +5629,25 @@
       <c r="T44" s="26"/>
       <c r="U44" s="26"/>
     </row>
-    <row r="45" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="26"/>
-      <c r="B45" s="26"/>
-      <c r="C45" s="26"/>
-      <c r="D45" s="26"/>
-      <c r="E45" s="26"/>
-      <c r="F45" s="28"/>
+    <row r="45" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="B45" s="34" t="s">
+        <v>155</v>
+      </c>
+      <c r="C45" s="21" t="s">
+        <v>157</v>
+      </c>
+      <c r="D45" s="17" t="s">
+        <v>180</v>
+      </c>
+      <c r="E45" s="18" t="s">
+        <v>181</v>
+      </c>
+      <c r="F45" s="9" t="s">
+        <v>279</v>
+      </c>
       <c r="G45" s="26"/>
       <c r="H45" s="26"/>
       <c r="I45" s="26"/>
@@ -5205,13 +5664,25 @@
       <c r="T45" s="26"/>
       <c r="U45" s="26"/>
     </row>
-    <row r="46" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="26"/>
-      <c r="B46" s="26"/>
-      <c r="C46" s="26"/>
-      <c r="D46" s="26"/>
-      <c r="E46" s="26"/>
-      <c r="F46" s="28"/>
+    <row r="46" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="B46" s="34" t="s">
+        <v>281</v>
+      </c>
+      <c r="C46" s="21" t="s">
+        <v>324</v>
+      </c>
+      <c r="D46" s="21" t="s">
+        <v>325</v>
+      </c>
+      <c r="E46" s="21" t="s">
+        <v>190</v>
+      </c>
+      <c r="F46" s="9" t="s">
+        <v>279</v>
+      </c>
       <c r="G46" s="26"/>
       <c r="H46" s="26"/>
       <c r="I46" s="26"/>
@@ -5228,13 +5699,25 @@
       <c r="T46" s="26"/>
       <c r="U46" s="26"/>
     </row>
-    <row r="47" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="26"/>
-      <c r="B47" s="26"/>
-      <c r="C47" s="26"/>
-      <c r="D47" s="26"/>
-      <c r="E47" s="26"/>
-      <c r="F47" s="28"/>
+    <row r="47" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="B47" s="34" t="s">
+        <v>282</v>
+      </c>
+      <c r="C47" s="21" t="s">
+        <v>368</v>
+      </c>
+      <c r="D47" s="21" t="s">
+        <v>326</v>
+      </c>
+      <c r="E47" s="21" t="s">
+        <v>190</v>
+      </c>
+      <c r="F47" s="9" t="s">
+        <v>279</v>
+      </c>
       <c r="G47" s="26"/>
       <c r="H47" s="26"/>
       <c r="I47" s="26"/>
@@ -5251,13 +5734,25 @@
       <c r="T47" s="26"/>
       <c r="U47" s="26"/>
     </row>
-    <row r="48" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="26"/>
-      <c r="B48" s="26"/>
-      <c r="C48" s="26"/>
-      <c r="D48" s="26"/>
-      <c r="E48" s="26"/>
-      <c r="F48" s="28"/>
+    <row r="48" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="B48" s="34" t="s">
+        <v>283</v>
+      </c>
+      <c r="C48" s="21" t="s">
+        <v>369</v>
+      </c>
+      <c r="D48" s="21" t="s">
+        <v>327</v>
+      </c>
+      <c r="E48" s="21" t="s">
+        <v>190</v>
+      </c>
+      <c r="F48" s="9" t="s">
+        <v>279</v>
+      </c>
       <c r="G48" s="26"/>
       <c r="H48" s="26"/>
       <c r="I48" s="26"/>
@@ -5274,13 +5769,25 @@
       <c r="T48" s="26"/>
       <c r="U48" s="26"/>
     </row>
-    <row r="49" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="26"/>
-      <c r="B49" s="26"/>
-      <c r="C49" s="26"/>
-      <c r="D49" s="26"/>
-      <c r="E49" s="26"/>
-      <c r="F49" s="28"/>
+    <row r="49" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="B49" s="34" t="s">
+        <v>284</v>
+      </c>
+      <c r="C49" s="21" t="s">
+        <v>370</v>
+      </c>
+      <c r="D49" s="35" t="s">
+        <v>328</v>
+      </c>
+      <c r="E49" s="21" t="s">
+        <v>190</v>
+      </c>
+      <c r="F49" s="9" t="s">
+        <v>279</v>
+      </c>
       <c r="G49" s="26"/>
       <c r="H49" s="26"/>
       <c r="I49" s="26"/>
@@ -5297,13 +5804,25 @@
       <c r="T49" s="26"/>
       <c r="U49" s="26"/>
     </row>
-    <row r="50" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="26"/>
-      <c r="B50" s="26"/>
-      <c r="C50" s="26"/>
-      <c r="D50" s="26"/>
-      <c r="E50" s="26"/>
-      <c r="F50" s="28"/>
+    <row r="50" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="B50" s="34" t="s">
+        <v>285</v>
+      </c>
+      <c r="C50" s="21" t="s">
+        <v>371</v>
+      </c>
+      <c r="D50" s="21" t="s">
+        <v>329</v>
+      </c>
+      <c r="E50" s="21" t="s">
+        <v>190</v>
+      </c>
+      <c r="F50" s="9" t="s">
+        <v>279</v>
+      </c>
       <c r="G50" s="26"/>
       <c r="H50" s="26"/>
       <c r="I50" s="26"/>
@@ -5320,13 +5839,25 @@
       <c r="T50" s="26"/>
       <c r="U50" s="26"/>
     </row>
-    <row r="51" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="26"/>
-      <c r="B51" s="26"/>
-      <c r="C51" s="26"/>
-      <c r="D51" s="26"/>
-      <c r="E51" s="26"/>
-      <c r="F51" s="28"/>
+    <row r="51" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="B51" s="34" t="s">
+        <v>286</v>
+      </c>
+      <c r="C51" s="21" t="s">
+        <v>372</v>
+      </c>
+      <c r="D51" s="35" t="s">
+        <v>330</v>
+      </c>
+      <c r="E51" s="21" t="s">
+        <v>190</v>
+      </c>
+      <c r="F51" s="9" t="s">
+        <v>279</v>
+      </c>
       <c r="G51" s="26"/>
       <c r="H51" s="26"/>
       <c r="I51" s="26"/>
@@ -5343,13 +5874,25 @@
       <c r="T51" s="26"/>
       <c r="U51" s="26"/>
     </row>
-    <row r="52" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="26"/>
-      <c r="B52" s="26"/>
-      <c r="C52" s="26"/>
-      <c r="D52" s="26"/>
-      <c r="E52" s="26"/>
-      <c r="F52" s="28"/>
+    <row r="52" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="B52" s="34" t="s">
+        <v>287</v>
+      </c>
+      <c r="C52" s="21" t="s">
+        <v>373</v>
+      </c>
+      <c r="D52" s="35" t="s">
+        <v>331</v>
+      </c>
+      <c r="E52" s="21" t="s">
+        <v>190</v>
+      </c>
+      <c r="F52" s="9" t="s">
+        <v>279</v>
+      </c>
       <c r="G52" s="26"/>
       <c r="H52" s="26"/>
       <c r="I52" s="26"/>
@@ -5366,13 +5909,25 @@
       <c r="T52" s="26"/>
       <c r="U52" s="26"/>
     </row>
-    <row r="53" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="26"/>
-      <c r="B53" s="26"/>
-      <c r="C53" s="26"/>
-      <c r="D53" s="26"/>
-      <c r="E53" s="26"/>
-      <c r="F53" s="28"/>
+    <row r="53" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="B53" s="34" t="s">
+        <v>288</v>
+      </c>
+      <c r="C53" s="21" t="s">
+        <v>374</v>
+      </c>
+      <c r="D53" s="35" t="s">
+        <v>332</v>
+      </c>
+      <c r="E53" s="21" t="s">
+        <v>190</v>
+      </c>
+      <c r="F53" s="9" t="s">
+        <v>279</v>
+      </c>
       <c r="G53" s="26"/>
       <c r="H53" s="26"/>
       <c r="I53" s="26"/>
@@ -5389,13 +5944,25 @@
       <c r="T53" s="26"/>
       <c r="U53" s="26"/>
     </row>
-    <row r="54" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="26"/>
-      <c r="B54" s="26"/>
-      <c r="C54" s="26"/>
-      <c r="D54" s="26"/>
-      <c r="E54" s="26"/>
-      <c r="F54" s="28"/>
+    <row r="54" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="B54" s="34" t="s">
+        <v>289</v>
+      </c>
+      <c r="C54" s="21" t="s">
+        <v>375</v>
+      </c>
+      <c r="D54" s="35" t="s">
+        <v>333</v>
+      </c>
+      <c r="E54" s="21" t="s">
+        <v>190</v>
+      </c>
+      <c r="F54" s="9" t="s">
+        <v>279</v>
+      </c>
       <c r="G54" s="26"/>
       <c r="H54" s="26"/>
       <c r="I54" s="26"/>
@@ -5412,13 +5979,25 @@
       <c r="T54" s="26"/>
       <c r="U54" s="26"/>
     </row>
-    <row r="55" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="26"/>
-      <c r="B55" s="26"/>
-      <c r="C55" s="26"/>
-      <c r="D55" s="26"/>
-      <c r="E55" s="26"/>
-      <c r="F55" s="28"/>
+    <row r="55" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="B55" s="34" t="s">
+        <v>290</v>
+      </c>
+      <c r="C55" s="21" t="s">
+        <v>376</v>
+      </c>
+      <c r="D55" s="35" t="s">
+        <v>334</v>
+      </c>
+      <c r="E55" s="21" t="s">
+        <v>190</v>
+      </c>
+      <c r="F55" s="9" t="s">
+        <v>279</v>
+      </c>
       <c r="G55" s="26"/>
       <c r="H55" s="26"/>
       <c r="I55" s="26"/>
@@ -5435,13 +6014,25 @@
       <c r="T55" s="26"/>
       <c r="U55" s="26"/>
     </row>
-    <row r="56" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="26"/>
-      <c r="B56" s="26"/>
-      <c r="C56" s="26"/>
-      <c r="D56" s="26"/>
-      <c r="E56" s="26"/>
-      <c r="F56" s="28"/>
+    <row r="56" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="B56" s="34" t="s">
+        <v>291</v>
+      </c>
+      <c r="C56" s="21" t="s">
+        <v>377</v>
+      </c>
+      <c r="D56" s="35" t="s">
+        <v>335</v>
+      </c>
+      <c r="E56" s="21" t="s">
+        <v>190</v>
+      </c>
+      <c r="F56" s="9" t="s">
+        <v>279</v>
+      </c>
       <c r="G56" s="26"/>
       <c r="H56" s="26"/>
       <c r="I56" s="26"/>
@@ -5458,13 +6049,25 @@
       <c r="T56" s="26"/>
       <c r="U56" s="26"/>
     </row>
-    <row r="57" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="26"/>
-      <c r="B57" s="26"/>
-      <c r="C57" s="26"/>
-      <c r="D57" s="26"/>
-      <c r="E57" s="26"/>
-      <c r="F57" s="28"/>
+    <row r="57" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="B57" s="34" t="s">
+        <v>292</v>
+      </c>
+      <c r="C57" s="21" t="s">
+        <v>378</v>
+      </c>
+      <c r="D57" s="35" t="s">
+        <v>336</v>
+      </c>
+      <c r="E57" s="21" t="s">
+        <v>190</v>
+      </c>
+      <c r="F57" s="9" t="s">
+        <v>279</v>
+      </c>
       <c r="G57" s="26"/>
       <c r="H57" s="26"/>
       <c r="I57" s="26"/>
@@ -5481,13 +6084,25 @@
       <c r="T57" s="26"/>
       <c r="U57" s="26"/>
     </row>
-    <row r="58" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="26"/>
-      <c r="B58" s="26"/>
-      <c r="C58" s="26"/>
-      <c r="D58" s="26"/>
-      <c r="E58" s="26"/>
-      <c r="F58" s="28"/>
+    <row r="58" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="B58" s="34" t="s">
+        <v>293</v>
+      </c>
+      <c r="C58" s="21" t="s">
+        <v>379</v>
+      </c>
+      <c r="D58" s="35" t="s">
+        <v>337</v>
+      </c>
+      <c r="E58" s="21" t="s">
+        <v>190</v>
+      </c>
+      <c r="F58" s="9" t="s">
+        <v>279</v>
+      </c>
       <c r="G58" s="26"/>
       <c r="H58" s="26"/>
       <c r="I58" s="26"/>
@@ -5504,13 +6119,25 @@
       <c r="T58" s="26"/>
       <c r="U58" s="26"/>
     </row>
-    <row r="59" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="26"/>
-      <c r="B59" s="26"/>
-      <c r="C59" s="26"/>
-      <c r="D59" s="26"/>
-      <c r="E59" s="26"/>
-      <c r="F59" s="28"/>
+    <row r="59" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="B59" s="34" t="s">
+        <v>294</v>
+      </c>
+      <c r="C59" s="21" t="s">
+        <v>380</v>
+      </c>
+      <c r="D59" s="35" t="s">
+        <v>338</v>
+      </c>
+      <c r="E59" s="21" t="s">
+        <v>190</v>
+      </c>
+      <c r="F59" s="9" t="s">
+        <v>279</v>
+      </c>
       <c r="G59" s="26"/>
       <c r="H59" s="26"/>
       <c r="I59" s="26"/>
@@ -5527,13 +6154,25 @@
       <c r="T59" s="26"/>
       <c r="U59" s="26"/>
     </row>
-    <row r="60" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="26"/>
-      <c r="B60" s="26"/>
-      <c r="C60" s="26"/>
-      <c r="D60" s="26"/>
-      <c r="E60" s="26"/>
-      <c r="F60" s="28"/>
+    <row r="60" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="B60" s="34" t="s">
+        <v>295</v>
+      </c>
+      <c r="C60" s="21" t="s">
+        <v>381</v>
+      </c>
+      <c r="D60" s="35" t="s">
+        <v>339</v>
+      </c>
+      <c r="E60" s="21" t="s">
+        <v>190</v>
+      </c>
+      <c r="F60" s="9" t="s">
+        <v>279</v>
+      </c>
       <c r="G60" s="26"/>
       <c r="H60" s="26"/>
       <c r="I60" s="26"/>
@@ -5550,13 +6189,25 @@
       <c r="T60" s="26"/>
       <c r="U60" s="26"/>
     </row>
-    <row r="61" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="26"/>
-      <c r="B61" s="26"/>
-      <c r="C61" s="26"/>
-      <c r="D61" s="26"/>
-      <c r="E61" s="26"/>
-      <c r="F61" s="28"/>
+    <row r="61" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="B61" s="34" t="s">
+        <v>296</v>
+      </c>
+      <c r="C61" s="21" t="s">
+        <v>382</v>
+      </c>
+      <c r="D61" s="35" t="s">
+        <v>340</v>
+      </c>
+      <c r="E61" s="21" t="s">
+        <v>190</v>
+      </c>
+      <c r="F61" s="9" t="s">
+        <v>279</v>
+      </c>
       <c r="G61" s="26"/>
       <c r="H61" s="26"/>
       <c r="I61" s="26"/>
@@ -5573,41 +6224,556 @@
       <c r="T61" s="26"/>
       <c r="U61" s="26"/>
     </row>
-    <row r="62" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="63" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="64" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="65" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="66" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="67" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="68" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="69" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="70" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="71" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="72" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="73" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="74" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="76" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="77" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="78" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="79" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="80" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="81" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="82" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="83" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="84" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="85" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="86" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="87" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="88" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="89" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="90" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="91" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="92" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="93" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="94" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="95" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="96" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="62" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="B62" s="34" t="s">
+        <v>297</v>
+      </c>
+      <c r="C62" s="21" t="s">
+        <v>383</v>
+      </c>
+      <c r="D62" s="35" t="s">
+        <v>341</v>
+      </c>
+      <c r="E62" s="21" t="s">
+        <v>190</v>
+      </c>
+      <c r="F62" s="9" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="63" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="B63" s="34" t="s">
+        <v>298</v>
+      </c>
+      <c r="C63" s="21" t="s">
+        <v>384</v>
+      </c>
+      <c r="D63" s="35" t="s">
+        <v>342</v>
+      </c>
+      <c r="E63" s="21" t="s">
+        <v>190</v>
+      </c>
+      <c r="F63" s="9" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="64" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="B64" s="34" t="s">
+        <v>299</v>
+      </c>
+      <c r="C64" s="21" t="s">
+        <v>385</v>
+      </c>
+      <c r="D64" s="35" t="s">
+        <v>343</v>
+      </c>
+      <c r="E64" s="21" t="s">
+        <v>190</v>
+      </c>
+      <c r="F64" s="9" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="B65" s="34" t="s">
+        <v>300</v>
+      </c>
+      <c r="C65" s="21" t="s">
+        <v>386</v>
+      </c>
+      <c r="D65" s="35" t="s">
+        <v>344</v>
+      </c>
+      <c r="E65" s="21" t="s">
+        <v>190</v>
+      </c>
+      <c r="F65" s="9" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="B66" s="34" t="s">
+        <v>301</v>
+      </c>
+      <c r="C66" s="21" t="s">
+        <v>387</v>
+      </c>
+      <c r="D66" s="35" t="s">
+        <v>345</v>
+      </c>
+      <c r="E66" s="21" t="s">
+        <v>190</v>
+      </c>
+      <c r="F66" s="9" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="B67" s="34" t="s">
+        <v>302</v>
+      </c>
+      <c r="C67" s="21" t="s">
+        <v>388</v>
+      </c>
+      <c r="D67" s="35" t="s">
+        <v>346</v>
+      </c>
+      <c r="E67" s="21" t="s">
+        <v>190</v>
+      </c>
+      <c r="F67" s="9" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="B68" s="34" t="s">
+        <v>303</v>
+      </c>
+      <c r="C68" s="21" t="s">
+        <v>389</v>
+      </c>
+      <c r="D68" s="35" t="s">
+        <v>347</v>
+      </c>
+      <c r="E68" s="21" t="s">
+        <v>190</v>
+      </c>
+      <c r="F68" s="9" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="B69" s="34" t="s">
+        <v>304</v>
+      </c>
+      <c r="C69" s="21" t="s">
+        <v>390</v>
+      </c>
+      <c r="D69" s="35" t="s">
+        <v>348</v>
+      </c>
+      <c r="E69" s="21" t="s">
+        <v>190</v>
+      </c>
+      <c r="F69" s="9" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="B70" s="34" t="s">
+        <v>305</v>
+      </c>
+      <c r="C70" s="21" t="s">
+        <v>391</v>
+      </c>
+      <c r="D70" s="35" t="s">
+        <v>349</v>
+      </c>
+      <c r="E70" s="21" t="s">
+        <v>190</v>
+      </c>
+      <c r="F70" s="9" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="B71" s="34" t="s">
+        <v>306</v>
+      </c>
+      <c r="C71" s="21" t="s">
+        <v>392</v>
+      </c>
+      <c r="D71" s="35" t="s">
+        <v>350</v>
+      </c>
+      <c r="E71" s="21" t="s">
+        <v>190</v>
+      </c>
+      <c r="F71" s="9" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="B72" s="34" t="s">
+        <v>307</v>
+      </c>
+      <c r="C72" s="21" t="s">
+        <v>393</v>
+      </c>
+      <c r="D72" s="35" t="s">
+        <v>351</v>
+      </c>
+      <c r="E72" s="21" t="s">
+        <v>190</v>
+      </c>
+      <c r="F72" s="9" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="B73" s="34" t="s">
+        <v>308</v>
+      </c>
+      <c r="C73" s="21" t="s">
+        <v>394</v>
+      </c>
+      <c r="D73" s="35" t="s">
+        <v>352</v>
+      </c>
+      <c r="E73" s="21" t="s">
+        <v>190</v>
+      </c>
+      <c r="F73" s="9" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="B74" s="34" t="s">
+        <v>309</v>
+      </c>
+      <c r="C74" s="21" t="s">
+        <v>395</v>
+      </c>
+      <c r="D74" s="35" t="s">
+        <v>353</v>
+      </c>
+      <c r="E74" s="21" t="s">
+        <v>190</v>
+      </c>
+      <c r="F74" s="9" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="B75" s="34" t="s">
+        <v>310</v>
+      </c>
+      <c r="C75" s="21" t="s">
+        <v>396</v>
+      </c>
+      <c r="D75" s="35" t="s">
+        <v>354</v>
+      </c>
+      <c r="E75" s="21" t="s">
+        <v>190</v>
+      </c>
+      <c r="F75" s="9" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="B76" s="34" t="s">
+        <v>311</v>
+      </c>
+      <c r="C76" s="21" t="s">
+        <v>397</v>
+      </c>
+      <c r="D76" s="35" t="s">
+        <v>355</v>
+      </c>
+      <c r="E76" s="21" t="s">
+        <v>190</v>
+      </c>
+      <c r="F76" s="9" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="B77" s="34" t="s">
+        <v>312</v>
+      </c>
+      <c r="C77" s="21" t="s">
+        <v>398</v>
+      </c>
+      <c r="D77" s="35" t="s">
+        <v>356</v>
+      </c>
+      <c r="E77" s="21" t="s">
+        <v>190</v>
+      </c>
+      <c r="F77" s="9" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="B78" s="34" t="s">
+        <v>313</v>
+      </c>
+      <c r="C78" s="21" t="s">
+        <v>399</v>
+      </c>
+      <c r="D78" s="35" t="s">
+        <v>357</v>
+      </c>
+      <c r="E78" s="21" t="s">
+        <v>190</v>
+      </c>
+      <c r="F78" s="9" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="B79" s="34" t="s">
+        <v>314</v>
+      </c>
+      <c r="C79" s="21" t="s">
+        <v>400</v>
+      </c>
+      <c r="D79" s="35" t="s">
+        <v>358</v>
+      </c>
+      <c r="E79" s="21" t="s">
+        <v>190</v>
+      </c>
+      <c r="F79" s="9" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="B80" s="34" t="s">
+        <v>315</v>
+      </c>
+      <c r="C80" s="21" t="s">
+        <v>401</v>
+      </c>
+      <c r="D80" s="35" t="s">
+        <v>359</v>
+      </c>
+      <c r="E80" s="21" t="s">
+        <v>190</v>
+      </c>
+      <c r="F80" s="9" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="B81" s="34" t="s">
+        <v>316</v>
+      </c>
+      <c r="C81" s="21" t="s">
+        <v>402</v>
+      </c>
+      <c r="D81" s="35" t="s">
+        <v>360</v>
+      </c>
+      <c r="E81" s="21" t="s">
+        <v>190</v>
+      </c>
+      <c r="F81" s="9" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="B82" s="34" t="s">
+        <v>317</v>
+      </c>
+      <c r="C82" s="21" t="s">
+        <v>403</v>
+      </c>
+      <c r="D82" s="35" t="s">
+        <v>361</v>
+      </c>
+      <c r="E82" s="21" t="s">
+        <v>190</v>
+      </c>
+      <c r="F82" s="9" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="B83" s="34" t="s">
+        <v>318</v>
+      </c>
+      <c r="C83" s="21" t="s">
+        <v>404</v>
+      </c>
+      <c r="D83" s="35" t="s">
+        <v>362</v>
+      </c>
+      <c r="E83" s="21" t="s">
+        <v>190</v>
+      </c>
+      <c r="F83" s="9" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="B84" s="34" t="s">
+        <v>319</v>
+      </c>
+      <c r="C84" s="21" t="s">
+        <v>405</v>
+      </c>
+      <c r="D84" s="35" t="s">
+        <v>363</v>
+      </c>
+      <c r="E84" s="21" t="s">
+        <v>190</v>
+      </c>
+      <c r="F84" s="9" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="B85" s="34" t="s">
+        <v>320</v>
+      </c>
+      <c r="C85" s="21" t="s">
+        <v>406</v>
+      </c>
+      <c r="D85" s="35" t="s">
+        <v>364</v>
+      </c>
+      <c r="E85" s="21" t="s">
+        <v>190</v>
+      </c>
+      <c r="F85" s="9" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="B86" s="34" t="s">
+        <v>321</v>
+      </c>
+      <c r="C86" s="21" t="s">
+        <v>407</v>
+      </c>
+      <c r="D86" s="35" t="s">
+        <v>365</v>
+      </c>
+      <c r="E86" s="21" t="s">
+        <v>190</v>
+      </c>
+      <c r="F86" s="9" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="B87" s="34" t="s">
+        <v>322</v>
+      </c>
+      <c r="C87" s="21" t="s">
+        <v>408</v>
+      </c>
+      <c r="D87" s="35" t="s">
+        <v>366</v>
+      </c>
+      <c r="E87" s="21" t="s">
+        <v>190</v>
+      </c>
+      <c r="F87" s="9" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="B88" s="34" t="s">
+        <v>323</v>
+      </c>
+      <c r="C88" s="21" t="s">
+        <v>409</v>
+      </c>
+      <c r="D88" s="35" t="s">
+        <v>367</v>
+      </c>
+      <c r="E88" s="21" t="s">
+        <v>190</v>
+      </c>
+      <c r="F88" s="9" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B89" s="18"/>
+    </row>
+    <row r="90" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="91" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="92" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="93" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="94" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="95" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="96" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="97" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="98" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="99" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6520,6 +7686,9 @@
     <row r="1006" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1007" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1008" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1048576" spans="5:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E1048576" s="21"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A2:F2"/>
@@ -6555,13 +7724,13 @@
       <c r="B1" s="6"/>
     </row>
     <row r="2" spans="1:19" ht="37" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="31" t="s">
         <v>140</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
     </row>
     <row r="3" spans="1:19" ht="38" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
@@ -8573,8 +9742,8 @@
   </sheetPr>
   <dimension ref="A1:S997"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:D8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -8591,13 +9760,13 @@
       <c r="B1" s="6"/>
     </row>
     <row r="2" spans="1:19" ht="37" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="31" t="s">
         <v>144</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
     </row>
     <row r="3" spans="1:19" ht="38" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
@@ -8766,10 +9935,18 @@
       <c r="S8" s="2"/>
     </row>
     <row r="9" spans="1:19" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
+      <c r="A9" s="13">
+        <v>45446</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>258</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>259</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>152</v>
+      </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>

</xml_diff>

<commit_message>
add region and income group to energy dataset
</commit_message>
<xml_diff>
--- a/course-datasets/Data dictionary.xlsx
+++ b/course-datasets/Data dictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stepheaneff/Documents/work/GT/data-science-basics-2024/course-datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{329C92E2-32E4-004B-8097-65CCAA30DC3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{159A91F7-DAD2-5A48-87E3-732900A67DDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="460" yWindow="760" windowWidth="29780" windowHeight="16820" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="460" yWindow="760" windowWidth="29780" windowHeight="16820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table information" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="738" uniqueCount="410">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="754" uniqueCount="413">
   <si>
     <t>Text</t>
   </si>
@@ -834,8 +834,443 @@
     <t>World Health Organization. (5 April, 2024).Measles-containing-vaccine first-dose (MCV1) immunization coverage among 1-year-olds (%). https://www.who.int/data/gho/data/indicators/indicator-details/GHO/measles-containing-vaccine-first-dose-(mcv1)</t>
   </si>
   <si>
+    <t>ico_code</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>is_latest_year</t>
+  </si>
+  <si>
+    <t>MCV1 coverage</t>
+  </si>
+  <si>
+    <t>Is latest year</t>
+  </si>
+  <si>
+    <t>The region of the country as designated by the World Bank as of 2024</t>
+  </si>
+  <si>
+    <t>Indicates whether or not the year is the most recent year for which data are available in the dataset</t>
+  </si>
+  <si>
+    <t>logical</t>
+  </si>
+  <si>
+    <t>The year for which data are reported</t>
+  </si>
+  <si>
+    <t>Measles-containing-vaccine first-dose (MCV1) immunization coverage among 1-year-olds, as a percentage</t>
+  </si>
+  <si>
+    <t>World Bank. (29 March, 2024). World Bank Country and Lending Groups. https://datahelpdesk.worldbank.org/knowledgebase/articles/906519-world-bank-country-and-lending-groups. Data for Venezuela missing from this data source and manually added to input dataset based on information from https://publicadministration.un.org/egovkb/en-us/Data/Country-Information/id/188-Venezuela as of May 24, 2024</t>
+  </si>
+  <si>
+    <t>energy_2022.tsv</t>
+  </si>
+  <si>
+    <t>Country-level information related to energy supply and utilization, as of the year 2022</t>
+  </si>
+  <si>
+    <t>one row per country</t>
+  </si>
+  <si>
+    <t>Hannah Ritchie, Pablo Rosado and Max Roser (2023). “Energy”, OurWorldInData.org.  'https://ourworldindata.org/energy'</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>population</t>
+  </si>
+  <si>
+    <t>gdp</t>
+  </si>
+  <si>
+    <t>biofuel_elec_per_capita</t>
+  </si>
+  <si>
+    <t>biofuel_electricity</t>
+  </si>
+  <si>
+    <t>biofuel_share_elec</t>
+  </si>
+  <si>
+    <t>carbon_intensity_elec</t>
+  </si>
+  <si>
+    <t>coal_elec_per_capita</t>
+  </si>
+  <si>
+    <t>coal_electricity</t>
+  </si>
+  <si>
+    <t>coal_share_elec</t>
+  </si>
+  <si>
+    <t>electricity_demand</t>
+  </si>
+  <si>
+    <t>electricity_generation</t>
+  </si>
+  <si>
+    <t>fossil_elec_per_capita</t>
+  </si>
+  <si>
+    <t>fossil_electricity</t>
+  </si>
+  <si>
+    <t>fossil_share_elec</t>
+  </si>
+  <si>
+    <t>gas_elec_per_capita</t>
+  </si>
+  <si>
+    <t>gas_electricity</t>
+  </si>
+  <si>
+    <t>gas_share_elec</t>
+  </si>
+  <si>
+    <t>greenhouse_gas_emissions</t>
+  </si>
+  <si>
+    <t>hydro_elec_per_capita</t>
+  </si>
+  <si>
+    <t>hydro_electricity</t>
+  </si>
+  <si>
+    <t>hydro_share_elec</t>
+  </si>
+  <si>
+    <t>low_carbon_elec_per_capita</t>
+  </si>
+  <si>
+    <t>low_carbon_electricity</t>
+  </si>
+  <si>
+    <t>low_carbon_share_elec</t>
+  </si>
+  <si>
+    <t>net_elec_imports</t>
+  </si>
+  <si>
+    <t>net_elec_imports_share_demand</t>
+  </si>
+  <si>
+    <t>nuclear_elec_per_capita</t>
+  </si>
+  <si>
+    <t>nuclear_electricity</t>
+  </si>
+  <si>
+    <t>nuclear_share_elec</t>
+  </si>
+  <si>
+    <t>oil_elec_per_capita</t>
+  </si>
+  <si>
+    <t>oil_electricity</t>
+  </si>
+  <si>
+    <t>oil_share_elec</t>
+  </si>
+  <si>
+    <t>other_renewable_electricity</t>
+  </si>
+  <si>
+    <t>other_renewables_elec_per_capita</t>
+  </si>
+  <si>
+    <t>per_capita_electricity</t>
+  </si>
+  <si>
+    <t>renewables_elec_per_capita</t>
+  </si>
+  <si>
+    <t>renewables_electricity</t>
+  </si>
+  <si>
+    <t>renewables_share_elec</t>
+  </si>
+  <si>
+    <t>solar_electricity</t>
+  </si>
+  <si>
+    <t>solar_share_elec</t>
+  </si>
+  <si>
+    <t>wind_elec_per_capita</t>
+  </si>
+  <si>
+    <t>wind_electricity</t>
+  </si>
+  <si>
+    <t>wind_share_elec</t>
+  </si>
+  <si>
+    <t>Country population</t>
+  </si>
+  <si>
+    <t>Population - Population by country, available from 10,000 BCE to 2100, based on data and estimates from different sources.</t>
+  </si>
+  <si>
+    <t>Gross domestic product (GDP) - This data is adjusted for inflation and differences in the cost of living between countries.</t>
+  </si>
+  <si>
+    <t>Electricity generation from bioenergy per person - Measured in kilowatt-hours per person.</t>
+  </si>
+  <si>
+    <t>Electricity generation from bioenergy - Measured in terawatt-hours.</t>
+  </si>
+  <si>
+    <t>Share of electricity generated by bioenergy - Measured as a percentage of total electricity.</t>
+  </si>
+  <si>
+    <t>Carbon intensity of electricity generation - Greenhouse gases emitted per unit of generated electricity, measured in grams of CO₂ equivalents per kilowatt-hour.</t>
+  </si>
+  <si>
+    <t>Electricity generation from coal per person - Measured in kilowatt-hours per person.</t>
+  </si>
+  <si>
+    <t>Electricity generation from coal - Measured in terawatt-hours.</t>
+  </si>
+  <si>
+    <t>Share of electricity generated by coal - Measured as a percentage of total electricity.</t>
+  </si>
+  <si>
+    <t>Electricity demand - Measured in terawatt-hours.</t>
+  </si>
+  <si>
+    <t>Total electricity generation - Measured in terawatt-hours.</t>
+  </si>
+  <si>
+    <t>Fossil fuel consumption per capita - Measured in kilowatt-hours per person.</t>
+  </si>
+  <si>
+    <t>Electricity generation from fossil fuels - Measured in terawatt-hours.</t>
+  </si>
+  <si>
+    <t>Share of electricity generated by fossil fuels - Measured as a percentage of total electricity.</t>
+  </si>
+  <si>
+    <t>Gas consumption per capita - Measured in kilowatt-hours per person.</t>
+  </si>
+  <si>
+    <t>Electricity generation from gas - Measured in terawatt-hours.</t>
+  </si>
+  <si>
+    <t>Share of electricity generated by gas - Measured as a percentage of total electricity.</t>
+  </si>
+  <si>
+    <t>Emissions from electricity generation - Measured in megatonnes of CO₂ equivalents.</t>
+  </si>
+  <si>
+    <t>Electricity generation from hydropower per person - Measured in kilowatt-hours per person.</t>
+  </si>
+  <si>
+    <t>Electricity generation from hydropower - Measured in terawatt-hours.</t>
+  </si>
+  <si>
+    <t>Share of electricity generated by hydropower - Measured as a percentage of total electricity.</t>
+  </si>
+  <si>
+    <t>Low-carbon energy consumption per capita - Measured in kilowatt-hours per person.</t>
+  </si>
+  <si>
+    <t>Electricity generation from low-carbon sources - Low-carbon sources correspond to renewables and nuclear power, that produce significantly less greenhouse-gas emissions than fossil fuels.</t>
+  </si>
+  <si>
+    <t>Share of electricity generated by low-carbon sources - Low-carbon sources correspond to renewables and nuclear power, that produce significantly less greenhouse-gas emissions than fossil fuels.</t>
+  </si>
+  <si>
+    <t>Net electricity imports - Electricity imports minus exports, measured in TWh.</t>
+  </si>
+  <si>
+    <t>Net electricity imports as a share of demand - Electricity imports minus exports, measured as a percentage of total electricity demand.</t>
+  </si>
+  <si>
+    <t>Electricity generation from nuclear power per person - Measured in kilowatt-hours per person.</t>
+  </si>
+  <si>
+    <t>Electricity generation from nuclear - Measured in terawatt-hours.</t>
+  </si>
+  <si>
+    <t>Share of electricity generated by nuclear power - Measured as a percentage of total electricity.</t>
+  </si>
+  <si>
+    <t>Electricity generation from oil per person - Measured in kilowatt-hours per person.</t>
+  </si>
+  <si>
+    <t>Electricity generation from oil - Measured in terawatt-hours.</t>
+  </si>
+  <si>
+    <t>Share of electricity generated by oil - Measured as a percentage of total electricity.</t>
+  </si>
+  <si>
+    <t>Electricity generation from other renewables, including bioenergy - Measured in terawatt-hours.</t>
+  </si>
+  <si>
+    <t>Electricity generation from other renewables, including bioenergy, per person - Measured in kilowatt-hours per person.</t>
+  </si>
+  <si>
+    <t>Total electricity generation per person - Measured in kilowatt-hours per person.</t>
+  </si>
+  <si>
+    <t>Electricity generation from renewables per person - Measured in kilowatt-hours per person.</t>
+  </si>
+  <si>
+    <t>Electricity generation from renewables - Measured in terawatt-hours.</t>
+  </si>
+  <si>
+    <t>Share of electricity generated by renewables - Measured as a percentage of total electricity.</t>
+  </si>
+  <si>
+    <t>Electricity generation from solar power - Measured in terawatt-hours.</t>
+  </si>
+  <si>
+    <t>Share of electricity generated by solar power - Measured as a percentage of total electricity.</t>
+  </si>
+  <si>
+    <t>Electricity generation from wind power per person - Measured in kilowatt-hours per person.</t>
+  </si>
+  <si>
+    <t>Electricity generation from wind power - Measured in terawatt-hours.</t>
+  </si>
+  <si>
+    <t>Share of electricity generated by wind power - Measured as a percentage of total electricity.</t>
+  </si>
+  <si>
+    <t>GDP</t>
+  </si>
+  <si>
+    <t>Electricity generation from bioenergy per person</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Electricity generation from bioenergy </t>
+  </si>
+  <si>
+    <t>Share of electricity generated by bioenergy</t>
+  </si>
+  <si>
+    <t>Carbon intensity of electricity generation</t>
+  </si>
+  <si>
+    <t>Electricity generation from coal per person</t>
+  </si>
+  <si>
+    <t>Electricity generation from coal</t>
+  </si>
+  <si>
+    <t>Share of electricity generated by coal</t>
+  </si>
+  <si>
+    <t>Electricity demand</t>
+  </si>
+  <si>
+    <t>Total electricity generation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fossil fuel consumption per capita </t>
+  </si>
+  <si>
+    <t>Electricity generation from fossil fuels</t>
+  </si>
+  <si>
+    <t>Share of electricity generated by fossil fuels</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gas consumption per capita </t>
+  </si>
+  <si>
+    <t>Electricity generation from gas</t>
+  </si>
+  <si>
+    <t>Share of electricity generated by gas</t>
+  </si>
+  <si>
+    <t>Emissions from electricity generation</t>
+  </si>
+  <si>
+    <t>Electricity generation from hydropower per person</t>
+  </si>
+  <si>
+    <t>Electricity generation from hydropower</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Share of electricity generated by hydropower </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Low-carbon energy consumption per capita </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Electricity generation from low-carbon sources </t>
+  </si>
+  <si>
+    <t>Share of electricity generated by low-carbon sources</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Net electricity imports </t>
+  </si>
+  <si>
+    <t>Net electricity imports as a share of demand</t>
+  </si>
+  <si>
+    <t>Electricity generation from nuclear power per person</t>
+  </si>
+  <si>
+    <t>Electricity generation from nuclear</t>
+  </si>
+  <si>
+    <t>Share of electricity generated by nuclear power</t>
+  </si>
+  <si>
+    <t>Electricity generation from oil per person</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Electricity generation from oil </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Share of electricity generated by oil </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Electricity generation from other renewables, including bioenergy </t>
+  </si>
+  <si>
+    <t>Electricity generation from other renewables, including bioenergy, per person</t>
+  </si>
+  <si>
+    <t>Total electricity generation per person</t>
+  </si>
+  <si>
+    <t>Electricity generation from renewables per person</t>
+  </si>
+  <si>
+    <t>Electricity generation from renewables</t>
+  </si>
+  <si>
+    <t>Share of electricity generated by renewables</t>
+  </si>
+  <si>
+    <t>Electricity generation from solar power</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Share of electricity generated by solar power </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Electricity generation from wind power per person </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Electricity generation from wind power </t>
+  </si>
+  <si>
+    <t>Share of electricity generated by wind power</t>
+  </si>
+  <si>
     <r>
-      <t xml:space="preserve">The data dictionary was last updated on </t>
+      <t xml:space="preserve">The data dictionary was last updated on June </t>
     </r>
     <r>
       <rPr>
@@ -844,443 +1279,17 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>May 24, 2024</t>
+      <t>4, 2024</t>
     </r>
   </si>
   <si>
-    <t>ico_code</t>
-  </si>
-  <si>
-    <t>year</t>
-  </si>
-  <si>
-    <t>is_latest_year</t>
-  </si>
-  <si>
-    <t>MCV1 coverage</t>
-  </si>
-  <si>
-    <t>Is latest year</t>
-  </si>
-  <si>
-    <t>The region of the country as designated by the World Bank as of 2024</t>
-  </si>
-  <si>
-    <t>Indicates whether or not the year is the most recent year for which data are available in the dataset</t>
-  </si>
-  <si>
-    <t>logical</t>
-  </si>
-  <si>
-    <t>The year for which data are reported</t>
-  </si>
-  <si>
-    <t>Measles-containing-vaccine first-dose (MCV1) immunization coverage among 1-year-olds, as a percentage</t>
-  </si>
-  <si>
-    <t>World Bank. (29 March, 2024). World Bank Country and Lending Groups. https://datahelpdesk.worldbank.org/knowledgebase/articles/906519-world-bank-country-and-lending-groups. Data for Venezuela missing from this data source and manually added to input dataset based on information from https://publicadministration.un.org/egovkb/en-us/Data/Country-Information/id/188-Venezuela as of May 24, 2024</t>
-  </si>
-  <si>
-    <t>energy_2022.tsv</t>
-  </si>
-  <si>
-    <t>Country-level information related to energy supply and utilization, as of the year 2022</t>
-  </si>
-  <si>
-    <t>one row per country</t>
-  </si>
-  <si>
-    <t>Hannah Ritchie, Pablo Rosado and Max Roser (2023). “Energy”, OurWorldInData.org.  'https://ourworldindata.org/energy'</t>
-  </si>
-  <si>
-    <t>country</t>
-  </si>
-  <si>
-    <t>population</t>
-  </si>
-  <si>
-    <t>gdp</t>
-  </si>
-  <si>
-    <t>biofuel_elec_per_capita</t>
-  </si>
-  <si>
-    <t>biofuel_electricity</t>
-  </si>
-  <si>
-    <t>biofuel_share_elec</t>
-  </si>
-  <si>
-    <t>carbon_intensity_elec</t>
-  </si>
-  <si>
-    <t>coal_elec_per_capita</t>
-  </si>
-  <si>
-    <t>coal_electricity</t>
-  </si>
-  <si>
-    <t>coal_share_elec</t>
-  </si>
-  <si>
-    <t>electricity_demand</t>
-  </si>
-  <si>
-    <t>electricity_generation</t>
-  </si>
-  <si>
-    <t>fossil_elec_per_capita</t>
-  </si>
-  <si>
-    <t>fossil_electricity</t>
-  </si>
-  <si>
-    <t>fossil_share_elec</t>
-  </si>
-  <si>
-    <t>gas_elec_per_capita</t>
-  </si>
-  <si>
-    <t>gas_electricity</t>
-  </si>
-  <si>
-    <t>gas_share_elec</t>
-  </si>
-  <si>
-    <t>greenhouse_gas_emissions</t>
-  </si>
-  <si>
-    <t>hydro_elec_per_capita</t>
-  </si>
-  <si>
-    <t>hydro_electricity</t>
-  </si>
-  <si>
-    <t>hydro_share_elec</t>
-  </si>
-  <si>
-    <t>low_carbon_elec_per_capita</t>
-  </si>
-  <si>
-    <t>low_carbon_electricity</t>
-  </si>
-  <si>
-    <t>low_carbon_share_elec</t>
-  </si>
-  <si>
-    <t>net_elec_imports</t>
-  </si>
-  <si>
-    <t>net_elec_imports_share_demand</t>
-  </si>
-  <si>
-    <t>nuclear_elec_per_capita</t>
-  </si>
-  <si>
-    <t>nuclear_electricity</t>
-  </si>
-  <si>
-    <t>nuclear_share_elec</t>
-  </si>
-  <si>
-    <t>oil_elec_per_capita</t>
-  </si>
-  <si>
-    <t>oil_electricity</t>
-  </si>
-  <si>
-    <t>oil_share_elec</t>
-  </si>
-  <si>
-    <t>other_renewable_electricity</t>
-  </si>
-  <si>
-    <t>other_renewables_elec_per_capita</t>
-  </si>
-  <si>
-    <t>per_capita_electricity</t>
-  </si>
-  <si>
-    <t>renewables_elec_per_capita</t>
-  </si>
-  <si>
-    <t>renewables_electricity</t>
-  </si>
-  <si>
-    <t>renewables_share_elec</t>
-  </si>
-  <si>
-    <t>solar_electricity</t>
-  </si>
-  <si>
-    <t>solar_share_elec</t>
-  </si>
-  <si>
-    <t>wind_elec_per_capita</t>
-  </si>
-  <si>
-    <t>wind_electricity</t>
-  </si>
-  <si>
-    <t>wind_share_elec</t>
-  </si>
-  <si>
-    <t>Country population</t>
-  </si>
-  <si>
-    <t>Population - Population by country, available from 10,000 BCE to 2100, based on data and estimates from different sources.</t>
-  </si>
-  <si>
-    <t>Gross domestic product (GDP) - This data is adjusted for inflation and differences in the cost of living between countries.</t>
-  </si>
-  <si>
-    <t>Electricity generation from bioenergy per person - Measured in kilowatt-hours per person.</t>
-  </si>
-  <si>
-    <t>Electricity generation from bioenergy - Measured in terawatt-hours.</t>
-  </si>
-  <si>
-    <t>Share of electricity generated by bioenergy - Measured as a percentage of total electricity.</t>
-  </si>
-  <si>
-    <t>Carbon intensity of electricity generation - Greenhouse gases emitted per unit of generated electricity, measured in grams of CO₂ equivalents per kilowatt-hour.</t>
-  </si>
-  <si>
-    <t>Electricity generation from coal per person - Measured in kilowatt-hours per person.</t>
-  </si>
-  <si>
-    <t>Electricity generation from coal - Measured in terawatt-hours.</t>
-  </si>
-  <si>
-    <t>Share of electricity generated by coal - Measured as a percentage of total electricity.</t>
-  </si>
-  <si>
-    <t>Electricity demand - Measured in terawatt-hours.</t>
-  </si>
-  <si>
-    <t>Total electricity generation - Measured in terawatt-hours.</t>
-  </si>
-  <si>
-    <t>Fossil fuel consumption per capita - Measured in kilowatt-hours per person.</t>
-  </si>
-  <si>
-    <t>Electricity generation from fossil fuels - Measured in terawatt-hours.</t>
-  </si>
-  <si>
-    <t>Share of electricity generated by fossil fuels - Measured as a percentage of total electricity.</t>
-  </si>
-  <si>
-    <t>Gas consumption per capita - Measured in kilowatt-hours per person.</t>
-  </si>
-  <si>
-    <t>Electricity generation from gas - Measured in terawatt-hours.</t>
-  </si>
-  <si>
-    <t>Share of electricity generated by gas - Measured as a percentage of total electricity.</t>
-  </si>
-  <si>
-    <t>Emissions from electricity generation - Measured in megatonnes of CO₂ equivalents.</t>
-  </si>
-  <si>
-    <t>Electricity generation from hydropower per person - Measured in kilowatt-hours per person.</t>
-  </si>
-  <si>
-    <t>Electricity generation from hydropower - Measured in terawatt-hours.</t>
-  </si>
-  <si>
-    <t>Share of electricity generated by hydropower - Measured as a percentage of total electricity.</t>
-  </si>
-  <si>
-    <t>Low-carbon energy consumption per capita - Measured in kilowatt-hours per person.</t>
-  </si>
-  <si>
-    <t>Electricity generation from low-carbon sources - Low-carbon sources correspond to renewables and nuclear power, that produce significantly less greenhouse-gas emissions than fossil fuels.</t>
-  </si>
-  <si>
-    <t>Share of electricity generated by low-carbon sources - Low-carbon sources correspond to renewables and nuclear power, that produce significantly less greenhouse-gas emissions than fossil fuels.</t>
-  </si>
-  <si>
-    <t>Net electricity imports - Electricity imports minus exports, measured in TWh.</t>
-  </si>
-  <si>
-    <t>Net electricity imports as a share of demand - Electricity imports minus exports, measured as a percentage of total electricity demand.</t>
-  </si>
-  <si>
-    <t>Electricity generation from nuclear power per person - Measured in kilowatt-hours per person.</t>
-  </si>
-  <si>
-    <t>Electricity generation from nuclear - Measured in terawatt-hours.</t>
-  </si>
-  <si>
-    <t>Share of electricity generated by nuclear power - Measured as a percentage of total electricity.</t>
-  </si>
-  <si>
-    <t>Electricity generation from oil per person - Measured in kilowatt-hours per person.</t>
-  </si>
-  <si>
-    <t>Electricity generation from oil - Measured in terawatt-hours.</t>
-  </si>
-  <si>
-    <t>Share of electricity generated by oil - Measured as a percentage of total electricity.</t>
-  </si>
-  <si>
-    <t>Electricity generation from other renewables, including bioenergy - Measured in terawatt-hours.</t>
-  </si>
-  <si>
-    <t>Electricity generation from other renewables, including bioenergy, per person - Measured in kilowatt-hours per person.</t>
-  </si>
-  <si>
-    <t>Total electricity generation per person - Measured in kilowatt-hours per person.</t>
-  </si>
-  <si>
-    <t>Electricity generation from renewables per person - Measured in kilowatt-hours per person.</t>
-  </si>
-  <si>
-    <t>Electricity generation from renewables - Measured in terawatt-hours.</t>
-  </si>
-  <si>
-    <t>Share of electricity generated by renewables - Measured as a percentage of total electricity.</t>
-  </si>
-  <si>
-    <t>Electricity generation from solar power - Measured in terawatt-hours.</t>
-  </si>
-  <si>
-    <t>Share of electricity generated by solar power - Measured as a percentage of total electricity.</t>
-  </si>
-  <si>
-    <t>Electricity generation from wind power per person - Measured in kilowatt-hours per person.</t>
-  </si>
-  <si>
-    <t>Electricity generation from wind power - Measured in terawatt-hours.</t>
-  </si>
-  <si>
-    <t>Share of electricity generated by wind power - Measured as a percentage of total electricity.</t>
-  </si>
-  <si>
-    <t>GDP</t>
-  </si>
-  <si>
-    <t>Electricity generation from bioenergy per person</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Electricity generation from bioenergy </t>
-  </si>
-  <si>
-    <t>Share of electricity generated by bioenergy</t>
-  </si>
-  <si>
-    <t>Carbon intensity of electricity generation</t>
-  </si>
-  <si>
-    <t>Electricity generation from coal per person</t>
-  </si>
-  <si>
-    <t>Electricity generation from coal</t>
-  </si>
-  <si>
-    <t>Share of electricity generated by coal</t>
-  </si>
-  <si>
-    <t>Electricity demand</t>
-  </si>
-  <si>
-    <t>Total electricity generation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fossil fuel consumption per capita </t>
-  </si>
-  <si>
-    <t>Electricity generation from fossil fuels</t>
-  </si>
-  <si>
-    <t>Share of electricity generated by fossil fuels</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gas consumption per capita </t>
-  </si>
-  <si>
-    <t>Electricity generation from gas</t>
-  </si>
-  <si>
-    <t>Share of electricity generated by gas</t>
-  </si>
-  <si>
-    <t>Emissions from electricity generation</t>
-  </si>
-  <si>
-    <t>Electricity generation from hydropower per person</t>
-  </si>
-  <si>
-    <t>Electricity generation from hydropower</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Share of electricity generated by hydropower </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Low-carbon energy consumption per capita </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Electricity generation from low-carbon sources </t>
-  </si>
-  <si>
-    <t>Share of electricity generated by low-carbon sources</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Net electricity imports </t>
-  </si>
-  <si>
-    <t>Net electricity imports as a share of demand</t>
-  </si>
-  <si>
-    <t>Electricity generation from nuclear power per person</t>
-  </si>
-  <si>
-    <t>Electricity generation from nuclear</t>
-  </si>
-  <si>
-    <t>Share of electricity generated by nuclear power</t>
-  </si>
-  <si>
-    <t>Electricity generation from oil per person</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Electricity generation from oil </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Share of electricity generated by oil </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Electricity generation from other renewables, including bioenergy </t>
-  </si>
-  <si>
-    <t>Electricity generation from other renewables, including bioenergy, per person</t>
-  </si>
-  <si>
-    <t>Total electricity generation per person</t>
-  </si>
-  <si>
-    <t>Electricity generation from renewables per person</t>
-  </si>
-  <si>
-    <t>Electricity generation from renewables</t>
-  </si>
-  <si>
-    <t>Share of electricity generated by renewables</t>
-  </si>
-  <si>
-    <t>Electricity generation from solar power</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Share of electricity generated by solar power </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Electricity generation from wind power per person </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Electricity generation from wind power </t>
-  </si>
-  <si>
-    <t>Share of electricity generated by wind power</t>
+    <t>Add additional fields to the energy dataset</t>
+  </si>
+  <si>
+    <t>New fields</t>
+  </si>
+  <si>
+    <t>World bank region and income group</t>
   </si>
 </sst>
 </file>
@@ -1810,8 +1819,8 @@
   </sheetPr>
   <dimension ref="A1:V1005"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1840,7 +1849,7 @@
     </row>
     <row r="3" spans="1:22" ht="17" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="30" t="s">
-        <v>264</v>
+        <v>409</v>
       </c>
       <c r="B3" s="30"/>
       <c r="C3" s="30"/>
@@ -1991,19 +2000,19 @@
     </row>
     <row r="11" spans="1:22" ht="100" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
+        <v>275</v>
+      </c>
+      <c r="B11" s="8" t="s">
         <v>276</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="C11" s="8" t="s">
         <v>277</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>278</v>
       </c>
       <c r="D11" s="9" t="s">
         <v>149</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
@@ -4142,7 +4151,7 @@
   <dimension ref="A1:U1048576"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E51" sqref="E51:E88"/>
+      <selection activeCell="C91" sqref="C91:G91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4349,7 +4358,7 @@
         <v>181</v>
       </c>
       <c r="F8" s="18" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="G8" s="26"/>
       <c r="H8" s="26"/>
@@ -4693,7 +4702,7 @@
         <v>209</v>
       </c>
       <c r="D18" s="17" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E18" s="18" t="s">
         <v>181</v>
@@ -4757,7 +4766,7 @@
         <v>260</v>
       </c>
       <c r="B20" s="20" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C20" s="20" t="s">
         <v>218</v>
@@ -4827,13 +4836,13 @@
         <v>260</v>
       </c>
       <c r="B22" s="20" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C22" s="21" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D22" s="21" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E22" s="21" t="s">
         <v>190</v>
@@ -4865,10 +4874,10 @@
         <v>200</v>
       </c>
       <c r="C23" s="21" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D23" s="21" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E23" s="21" t="s">
         <v>190</v>
@@ -4940,7 +4949,7 @@
         <v>209</v>
       </c>
       <c r="D25" s="17" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E25" s="18" t="s">
         <v>181</v>
@@ -5004,16 +5013,16 @@
         <v>260</v>
       </c>
       <c r="B27" s="20" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C27" s="21" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D27" s="21" t="s">
+        <v>270</v>
+      </c>
+      <c r="E27" s="21" t="s">
         <v>271</v>
-      </c>
-      <c r="E27" s="21" t="s">
-        <v>272</v>
       </c>
       <c r="F27" s="9" t="s">
         <v>263</v>
@@ -5596,10 +5605,10 @@
     </row>
     <row r="44" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="8" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B44" s="34" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C44" s="21" t="s">
         <v>216</v>
@@ -5611,7 +5620,7 @@
         <v>181</v>
       </c>
       <c r="F44" s="9" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="G44" s="26"/>
       <c r="H44" s="26"/>
@@ -5631,7 +5640,7 @@
     </row>
     <row r="45" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="8" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B45" s="34" t="s">
         <v>155</v>
@@ -5646,7 +5655,7 @@
         <v>181</v>
       </c>
       <c r="F45" s="9" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="G45" s="26"/>
       <c r="H45" s="26"/>
@@ -5666,22 +5675,22 @@
     </row>
     <row r="46" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="8" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B46" s="34" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C46" s="21" t="s">
+        <v>323</v>
+      </c>
+      <c r="D46" s="21" t="s">
         <v>324</v>
-      </c>
-      <c r="D46" s="21" t="s">
-        <v>325</v>
       </c>
       <c r="E46" s="21" t="s">
         <v>190</v>
       </c>
       <c r="F46" s="9" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="G46" s="26"/>
       <c r="H46" s="26"/>
@@ -5701,22 +5710,22 @@
     </row>
     <row r="47" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="8" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B47" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C47" s="21" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D47" s="21" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E47" s="21" t="s">
         <v>190</v>
       </c>
       <c r="F47" s="9" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="G47" s="26"/>
       <c r="H47" s="26"/>
@@ -5736,22 +5745,22 @@
     </row>
     <row r="48" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="8" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B48" s="34" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C48" s="21" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D48" s="21" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="E48" s="21" t="s">
         <v>190</v>
       </c>
       <c r="F48" s="9" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="G48" s="26"/>
       <c r="H48" s="26"/>
@@ -5771,22 +5780,22 @@
     </row>
     <row r="49" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="8" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B49" s="34" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C49" s="21" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D49" s="35" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="E49" s="21" t="s">
         <v>190</v>
       </c>
       <c r="F49" s="9" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="G49" s="26"/>
       <c r="H49" s="26"/>
@@ -5806,22 +5815,22 @@
     </row>
     <row r="50" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="8" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B50" s="34" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C50" s="21" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D50" s="21" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E50" s="21" t="s">
         <v>190</v>
       </c>
       <c r="F50" s="9" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="G50" s="26"/>
       <c r="H50" s="26"/>
@@ -5841,22 +5850,22 @@
     </row>
     <row r="51" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="8" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B51" s="34" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C51" s="21" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D51" s="35" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E51" s="21" t="s">
         <v>190</v>
       </c>
       <c r="F51" s="9" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="G51" s="26"/>
       <c r="H51" s="26"/>
@@ -5876,22 +5885,22 @@
     </row>
     <row r="52" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="8" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B52" s="34" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C52" s="21" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D52" s="35" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E52" s="21" t="s">
         <v>190</v>
       </c>
       <c r="F52" s="9" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="G52" s="26"/>
       <c r="H52" s="26"/>
@@ -5911,22 +5920,22 @@
     </row>
     <row r="53" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="8" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B53" s="34" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C53" s="21" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D53" s="35" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E53" s="21" t="s">
         <v>190</v>
       </c>
       <c r="F53" s="9" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="G53" s="26"/>
       <c r="H53" s="26"/>
@@ -5946,22 +5955,22 @@
     </row>
     <row r="54" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="8" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B54" s="34" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C54" s="21" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D54" s="35" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E54" s="21" t="s">
         <v>190</v>
       </c>
       <c r="F54" s="9" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="G54" s="26"/>
       <c r="H54" s="26"/>
@@ -5981,22 +5990,22 @@
     </row>
     <row r="55" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="8" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B55" s="34" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C55" s="21" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="D55" s="35" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E55" s="21" t="s">
         <v>190</v>
       </c>
       <c r="F55" s="9" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="G55" s="26"/>
       <c r="H55" s="26"/>
@@ -6016,22 +6025,22 @@
     </row>
     <row r="56" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="8" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B56" s="34" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C56" s="21" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D56" s="35" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E56" s="21" t="s">
         <v>190</v>
       </c>
       <c r="F56" s="9" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="G56" s="26"/>
       <c r="H56" s="26"/>
@@ -6051,22 +6060,22 @@
     </row>
     <row r="57" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="8" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B57" s="34" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C57" s="21" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D57" s="35" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E57" s="21" t="s">
         <v>190</v>
       </c>
       <c r="F57" s="9" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="G57" s="26"/>
       <c r="H57" s="26"/>
@@ -6086,22 +6095,22 @@
     </row>
     <row r="58" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="8" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B58" s="34" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C58" s="21" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="D58" s="35" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E58" s="21" t="s">
         <v>190</v>
       </c>
       <c r="F58" s="9" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="G58" s="26"/>
       <c r="H58" s="26"/>
@@ -6121,22 +6130,22 @@
     </row>
     <row r="59" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="8" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B59" s="34" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C59" s="21" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="D59" s="35" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E59" s="21" t="s">
         <v>190</v>
       </c>
       <c r="F59" s="9" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="G59" s="26"/>
       <c r="H59" s="26"/>
@@ -6156,22 +6165,22 @@
     </row>
     <row r="60" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="8" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B60" s="34" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C60" s="21" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D60" s="35" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="E60" s="21" t="s">
         <v>190</v>
       </c>
       <c r="F60" s="9" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="G60" s="26"/>
       <c r="H60" s="26"/>
@@ -6191,22 +6200,22 @@
     </row>
     <row r="61" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="8" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B61" s="34" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C61" s="21" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="D61" s="35" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="E61" s="21" t="s">
         <v>190</v>
       </c>
       <c r="F61" s="9" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="G61" s="26"/>
       <c r="H61" s="26"/>
@@ -6226,554 +6235,600 @@
     </row>
     <row r="62" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="8" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B62" s="34" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C62" s="21" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="D62" s="35" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E62" s="21" t="s">
         <v>190</v>
       </c>
       <c r="F62" s="9" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="63" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="8" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B63" s="34" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C63" s="21" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D63" s="35" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="E63" s="21" t="s">
         <v>190</v>
       </c>
       <c r="F63" s="9" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="64" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="8" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B64" s="34" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C64" s="21" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D64" s="35" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E64" s="21" t="s">
         <v>190</v>
       </c>
       <c r="F64" s="9" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="65" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="8" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B65" s="34" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C65" s="21" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D65" s="35" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E65" s="21" t="s">
         <v>190</v>
       </c>
       <c r="F65" s="9" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="66" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="8" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B66" s="34" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C66" s="21" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D66" s="35" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E66" s="21" t="s">
         <v>190</v>
       </c>
       <c r="F66" s="9" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="67" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="8" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B67" s="34" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C67" s="21" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D67" s="35" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E67" s="21" t="s">
         <v>190</v>
       </c>
       <c r="F67" s="9" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="68" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="8" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B68" s="34" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C68" s="21" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="D68" s="35" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E68" s="21" t="s">
         <v>190</v>
       </c>
       <c r="F68" s="9" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="8" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B69" s="34" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C69" s="21" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="D69" s="35" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="E69" s="21" t="s">
         <v>190</v>
       </c>
       <c r="F69" s="9" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="70" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="8" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B70" s="34" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C70" s="21" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D70" s="35" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E70" s="21" t="s">
         <v>190</v>
       </c>
       <c r="F70" s="9" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="71" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="8" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B71" s="34" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C71" s="21" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="D71" s="35" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="E71" s="21" t="s">
         <v>190</v>
       </c>
       <c r="F71" s="9" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="72" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="8" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B72" s="34" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C72" s="21" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D72" s="35" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="E72" s="21" t="s">
         <v>190</v>
       </c>
       <c r="F72" s="9" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="73" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="8" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B73" s="34" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C73" s="21" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D73" s="35" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E73" s="21" t="s">
         <v>190</v>
       </c>
       <c r="F73" s="9" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="74" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="8" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B74" s="34" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C74" s="21" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D74" s="35" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="E74" s="21" t="s">
         <v>190</v>
       </c>
       <c r="F74" s="9" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="75" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="8" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B75" s="34" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C75" s="21" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D75" s="35" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E75" s="21" t="s">
         <v>190</v>
       </c>
       <c r="F75" s="9" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="76" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="8" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B76" s="34" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C76" s="21" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="D76" s="35" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E76" s="21" t="s">
         <v>190</v>
       </c>
       <c r="F76" s="9" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="77" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="8" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B77" s="34" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C77" s="21" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="D77" s="35" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="E77" s="21" t="s">
         <v>190</v>
       </c>
       <c r="F77" s="9" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="78" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="8" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B78" s="34" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C78" s="21" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D78" s="35" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E78" s="21" t="s">
         <v>190</v>
       </c>
       <c r="F78" s="9" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="79" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="8" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B79" s="34" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C79" s="21" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D79" s="35" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E79" s="21" t="s">
         <v>190</v>
       </c>
       <c r="F79" s="9" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="80" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="8" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B80" s="34" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C80" s="21" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D80" s="35" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E80" s="21" t="s">
         <v>190</v>
       </c>
       <c r="F80" s="9" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.25">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" ht="50" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="8" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B81" s="34" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C81" s="21" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D81" s="35" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="E81" s="21" t="s">
         <v>190</v>
       </c>
       <c r="F81" s="9" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.25">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" ht="50" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="8" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B82" s="34" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C82" s="21" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="D82" s="35" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="E82" s="21" t="s">
         <v>190</v>
       </c>
       <c r="F82" s="9" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.25">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" ht="50" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="8" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B83" s="34" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C83" s="21" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="D83" s="35" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E83" s="21" t="s">
         <v>190</v>
       </c>
       <c r="F83" s="9" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.25">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" ht="50" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="8" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B84" s="34" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C84" s="21" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="D84" s="35" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E84" s="21" t="s">
         <v>190</v>
       </c>
       <c r="F84" s="9" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.25">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" ht="50" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="8" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B85" s="34" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C85" s="21" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="D85" s="35" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E85" s="21" t="s">
         <v>190</v>
       </c>
       <c r="F85" s="9" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.25">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" ht="50" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="8" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B86" s="34" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C86" s="21" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="D86" s="35" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E86" s="21" t="s">
         <v>190</v>
       </c>
       <c r="F86" s="9" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.25">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" ht="50" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="8" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B87" s="34" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C87" s="21" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="D87" s="35" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="E87" s="21" t="s">
         <v>190</v>
       </c>
       <c r="F87" s="9" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.25">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" ht="50" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="8" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B88" s="34" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C88" s="21" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="D88" s="35" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="E88" s="21" t="s">
         <v>190</v>
       </c>
       <c r="F88" s="9" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B89" s="18"/>
-    </row>
-    <row r="90" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="91" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="92" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="93" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="94" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="95" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="96" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+        <v>278</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" ht="50" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="8" t="s">
+        <v>275</v>
+      </c>
+      <c r="B89" s="34" t="s">
+        <v>161</v>
+      </c>
+      <c r="C89" s="21" t="s">
+        <v>167</v>
+      </c>
+      <c r="D89" s="17" t="s">
+        <v>189</v>
+      </c>
+      <c r="E89" s="18" t="s">
+        <v>181</v>
+      </c>
+      <c r="F89" s="18" t="s">
+        <v>274</v>
+      </c>
+      <c r="G89" s="26"/>
+      <c r="H89" s="26"/>
+    </row>
+    <row r="90" spans="1:8" ht="50" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="8" t="s">
+        <v>275</v>
+      </c>
+      <c r="B90" s="34" t="s">
+        <v>160</v>
+      </c>
+      <c r="C90" s="21" t="s">
+        <v>166</v>
+      </c>
+      <c r="D90" s="17" t="s">
+        <v>188</v>
+      </c>
+      <c r="E90" s="18" t="s">
+        <v>181</v>
+      </c>
+      <c r="F90" s="18" t="s">
+        <v>185</v>
+      </c>
+      <c r="G90" s="26"/>
+      <c r="H90" s="26"/>
+    </row>
+    <row r="91" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C91" s="21"/>
+      <c r="D91" s="17"/>
+      <c r="E91" s="18"/>
+      <c r="F91" s="18"/>
+      <c r="G91" s="26"/>
+    </row>
+    <row r="92" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="93" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="94" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="95" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="96" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="97" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="98" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="99" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -9742,8 +9797,8 @@
   </sheetPr>
   <dimension ref="A1:S997"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:D9"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -9964,11 +10019,21 @@
       <c r="S9" s="2"/>
     </row>
     <row r="10" spans="1:19" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
+      <c r="A10" s="13">
+        <v>45447</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>410</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>411</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>412</v>
+      </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>

</xml_diff>